<commit_message>
Introduced EIGENAAR as a demo owner
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="290">
   <si>
     <t>Name</t>
   </si>
@@ -892,6 +892,9 @@
   </si>
   <si>
     <t>NEN3610_GML321</t>
+  </si>
+  <si>
+    <t>click</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1033,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1123,6 +1126,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1423,10 +1432,10 @@
   <dimension ref="A1:Q125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1627,16 +1636,16 @@
       <c r="Q6"/>
     </row>
     <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="37" t="b">
+      <c r="D7" s="39" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
@@ -1651,10 +1660,10 @@
       <c r="Q7"/>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="G8" s="21"/>
       <c r="L8" s="21"/>
       <c r="M8" s="17"/>
@@ -2411,6 +2420,9 @@
       <c r="E32" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F32" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G32" s="21"/>
       <c r="L32" s="21"/>
       <c r="M32" s="17"/>
@@ -2435,6 +2447,9 @@
       <c r="E33" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F33" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="G33" s="21"/>
       <c r="L33" s="21"/>
       <c r="M33" s="17"/>
@@ -2619,16 +2634,16 @@
         <v>1</v>
       </c>
       <c r="G38" s="28"/>
-      <c r="H38" s="31" t="s">
+      <c r="H38" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I38" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="J38" s="33" t="s">
+      <c r="J38" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="33" t="s">
+      <c r="K38" s="38" t="s">
         <v>25</v>
       </c>
       <c r="L38" s="28"/>
@@ -2720,16 +2735,16 @@
       <c r="Q41"/>
     </row>
     <row r="42" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D42" s="37" t="b">
+      <c r="D42" s="39" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="2" t="b">
@@ -2747,10 +2762,10 @@
       <c r="Q42"/>
     </row>
     <row r="43" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
+      <c r="A43" s="39"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
       <c r="G43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="17"/>

</xml_diff>

<commit_message>
Demo [eigenaar] krijgt visuals
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="322">
   <si>
     <t>Name</t>
   </si>
@@ -985,6 +985,12 @@
   </si>
   <si>
     <t>LOGICAL: docrelease</t>
+  </si>
+  <si>
+    <t>visuals</t>
+  </si>
+  <si>
+    <t>Name of the visuals file</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1122,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1200,6 +1206,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1514,13 +1523,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S115"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
+      <selection pane="bottomRight" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1739,16 +1748,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="40" t="s">
+      <c r="C7" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="40" t="b">
+      <c r="D7" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -1768,10 +1777,10 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
       <c r="G8" s="18"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -3019,16 +3028,16 @@
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="40" t="b">
+      <c r="D45" s="41" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="b">
@@ -3051,10 +3060,10 @@
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
       <c r="G46" s="18"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
@@ -5144,59 +5153,74 @@
       <c r="Q112" s="25"/>
       <c r="R112"/>
     </row>
-    <row r="113" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:18" s="40" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A113" s="40" t="s">
+        <v>320</v>
+      </c>
+      <c r="B113" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="40" t="s">
+        <v>321</v>
+      </c>
+      <c r="D113" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="25"/>
+      <c r="H113" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="I113" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="J113" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="K113" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="L113" s="25"/>
+      <c r="M113" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="N113" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="O113" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="P113" s="40" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q113" s="25"/>
+    </row>
+    <row r="114" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A114" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B114" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C114" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D113" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F113" s="1" t="s">
+      <c r="D114" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G113" s="18"/>
-      <c r="H113" s="15"/>
-      <c r="I113" s="15"/>
-      <c r="J113" s="15"/>
-      <c r="K113" s="15"/>
-      <c r="L113" s="25"/>
-      <c r="M113" s="38"/>
-      <c r="N113" s="38"/>
-      <c r="O113" s="38"/>
-      <c r="P113" s="38"/>
-      <c r="Q113" s="25"/>
-      <c r="R113"/>
-    </row>
-    <row r="114" spans="1:18" s="23" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A114" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="B114" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C114" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="D114" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F114" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="G114" s="25"/>
-      <c r="H114" s="24"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+      <c r="J114" s="15"/>
+      <c r="K114" s="15"/>
       <c r="L114" s="25"/>
       <c r="M114" s="38"/>
       <c r="N114" s="38"/>
@@ -5205,30 +5229,27 @@
       <c r="Q114" s="25"/>
       <c r="R114"/>
     </row>
-    <row r="115" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A115" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D115" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G115" s="18"/>
-      <c r="H115" s="15"/>
-      <c r="I115" s="15"/>
-      <c r="J115" s="15"/>
-      <c r="K115" s="15"/>
+    <row r="115" spans="1:18" s="23" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A115" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B115" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C115" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="D115" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F115" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="G115" s="25"/>
+      <c r="H115" s="24"/>
       <c r="L115" s="25"/>
       <c r="M115" s="38"/>
       <c r="N115" s="38"/>
@@ -5236,6 +5257,38 @@
       <c r="P115" s="38"/>
       <c r="Q115" s="25"/>
       <c r="R115"/>
+    </row>
+    <row r="116" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A116" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D116" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G116" s="18"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="15"/>
+      <c r="J116" s="15"/>
+      <c r="K116" s="15"/>
+      <c r="L116" s="25"/>
+      <c r="M116" s="38"/>
+      <c r="N116" s="38"/>
+      <c r="O116" s="38"/>
+      <c r="P116" s="38"/>
+      <c r="Q116" s="25"/>
+      <c r="R116"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[EIGENAAR] Correcties basis config; naar MIM11.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="325">
   <si>
     <t>Name</t>
   </si>
@@ -991,6 +991,15 @@
   </si>
   <si>
     <t>Name of the visuals file</t>
+  </si>
+  <si>
+    <t>respec</t>
+  </si>
+  <si>
+    <t>fullrespec</t>
+  </si>
+  <si>
+    <t>Should a full respec version be generated along with the catalog?</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1131,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1206,6 +1215,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1523,13 +1538,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S116"/>
+  <dimension ref="A1:S117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G113" sqref="G113"/>
+      <selection pane="bottomRight" activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1748,16 +1763,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="41" t="b">
+      <c r="D7" s="43" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -1777,10 +1792,10 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
       <c r="G8" s="18"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -2703,11 +2718,31 @@
         <v>273</v>
       </c>
       <c r="G35" s="25"/>
+      <c r="H35" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="I35" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="K35" s="29" t="s">
+        <v>322</v>
+      </c>
       <c r="L35" s="25"/>
-      <c r="M35" s="38"/>
-      <c r="N35" s="38"/>
-      <c r="O35" s="38"/>
-      <c r="P35" s="38"/>
+      <c r="M35" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="N35" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="O35" s="41" t="s">
+        <v>322</v>
+      </c>
+      <c r="P35" s="41" t="s">
+        <v>322</v>
+      </c>
       <c r="Q35" s="25"/>
       <c r="R35"/>
     </row>
@@ -3028,16 +3063,16 @@
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="41" t="b">
+      <c r="D45" s="43" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="b">
@@ -3060,10 +3095,10 @@
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="G46" s="18"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>
@@ -3379,68 +3414,85 @@
       <c r="Q56" s="25"/>
       <c r="R56"/>
     </row>
-    <row r="57" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A57" s="14" t="s">
+    <row r="57" spans="1:18" s="42" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="42" t="s">
+        <v>323</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>324</v>
+      </c>
+      <c r="D57" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="42" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="25"/>
+      <c r="I57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="25"/>
+      <c r="N57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="42" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="25"/>
+    </row>
+    <row r="58" spans="1:18" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A58" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B58" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C58" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="D57" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="20"/>
-    </row>
-    <row r="58" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="D58" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="G58" s="25"/>
-      <c r="L58" s="25"/>
-      <c r="Q58" s="25"/>
-      <c r="R58"/>
+      <c r="D58" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="14"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="14"/>
+      <c r="O58" s="14"/>
+      <c r="P58" s="14"/>
+      <c r="Q58" s="20"/>
     </row>
     <row r="59" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>90</v>
+        <v>284</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D59" s="5" t="b">
         <v>0</v>
@@ -3448,29 +3500,23 @@
       <c r="E59" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F59" s="32"/>
+      <c r="F59" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="G59" s="25"/>
-      <c r="H59" s="32"/>
-      <c r="I59" s="32"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
       <c r="L59" s="25"/>
-      <c r="M59" s="32"/>
-      <c r="N59" s="32"/>
-      <c r="O59" s="32"/>
-      <c r="P59" s="32"/>
       <c r="Q59" s="25"/>
       <c r="R59"/>
     </row>
-    <row r="60" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A60" s="5" t="s">
-        <v>188</v>
+        <v>287</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>189</v>
+        <v>288</v>
       </c>
       <c r="D60" s="5" t="b">
         <v>0</v>
@@ -3478,29 +3524,35 @@
       <c r="E60" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="F60" s="32"/>
       <c r="G60" s="25"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
       <c r="L60" s="25"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
+      <c r="O60" s="32"/>
+      <c r="P60" s="32"/>
       <c r="Q60" s="25"/>
       <c r="R60"/>
     </row>
-    <row r="61" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>295</v>
-      </c>
-      <c r="B61" t="s">
-        <v>82</v>
-      </c>
-      <c r="C61" t="s">
-        <v>297</v>
-      </c>
-      <c r="D61" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" t="s">
-        <v>303</v>
+    <row r="61" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A61" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G61" s="25"/>
       <c r="L61" s="25"/>
@@ -3509,13 +3561,13 @@
     </row>
     <row r="62" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B62" t="s">
         <v>82</v>
       </c>
       <c r="C62" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D62" t="b">
         <v>0</v>
@@ -3524,120 +3576,116 @@
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="G62" s="25"/>
       <c r="L62" s="25"/>
       <c r="Q62" s="25"/>
       <c r="R62"/>
     </row>
-    <row r="63" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A63" s="14" t="s">
+    <row r="63" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>296</v>
+      </c>
+      <c r="B63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="s">
+        <v>298</v>
+      </c>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" t="s">
+        <v>299</v>
+      </c>
+      <c r="G63" s="25"/>
+      <c r="L63" s="25"/>
+      <c r="Q63" s="25"/>
+      <c r="R63"/>
+    </row>
+    <row r="64" spans="1:18" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A64" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B64" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C64" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="D63" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="14" t="s">
+      <c r="D64" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="G63" s="20"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
-      <c r="O63" s="14"/>
-      <c r="P63" s="14"/>
-      <c r="Q63" s="20"/>
-    </row>
-    <row r="64" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="5" t="s">
+      <c r="G64" s="20"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="20"/>
+      <c r="M64" s="14"/>
+      <c r="N64" s="14"/>
+      <c r="O64" s="14"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="20"/>
+    </row>
+    <row r="65" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A65" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B65" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="D64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F64" s="5" t="s">
+      <c r="D65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G64" s="18"/>
-      <c r="L64" s="25"/>
-      <c r="Q64" s="25"/>
-      <c r="R64"/>
-    </row>
-    <row r="65" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="G65" s="18"/>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
       <c r="L65" s="25"/>
-      <c r="M65" s="38"/>
-      <c r="N65" s="38"/>
-      <c r="O65" s="38"/>
-      <c r="P65" s="38"/>
       <c r="Q65" s="25"/>
       <c r="R65"/>
     </row>
-    <row r="66" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>290</v>
-      </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="D66" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="G66" s="25"/>
+    <row r="66" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G66" s="18"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
       <c r="L66" s="25"/>
       <c r="M66" s="38"/>
       <c r="N66" s="38"/>
@@ -3646,95 +3694,91 @@
       <c r="Q66" s="25"/>
       <c r="R66"/>
     </row>
-    <row r="67" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G67" s="18"/>
+    <row r="67" spans="1:18" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>290</v>
+      </c>
+      <c r="B67" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="D67" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="25"/>
       <c r="L67" s="25"/>
+      <c r="M67" s="38"/>
+      <c r="N67" s="38"/>
+      <c r="O67" s="38"/>
+      <c r="P67" s="38"/>
       <c r="Q67" s="25"/>
       <c r="R67"/>
     </row>
     <row r="68" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>262</v>
-      </c>
-      <c r="B68" t="s">
-        <v>82</v>
-      </c>
-      <c r="C68" t="s">
-        <v>263</v>
-      </c>
-      <c r="D68" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" t="b">
-        <v>1</v>
-      </c>
-      <c r="F68" t="s">
-        <v>228</v>
-      </c>
-      <c r="G68" s="25"/>
+      <c r="A68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E68" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G68" s="18"/>
       <c r="L68" s="25"/>
       <c r="Q68" s="25"/>
       <c r="R68"/>
     </row>
-    <row r="69" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G69" s="18"/>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15"/>
+    <row r="69" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>262</v>
+      </c>
+      <c r="B69" t="s">
+        <v>82</v>
+      </c>
+      <c r="C69" t="s">
+        <v>263</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>228</v>
+      </c>
+      <c r="G69" s="25"/>
       <c r="L69" s="25"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
-      <c r="O69" s="38"/>
-      <c r="P69" s="38"/>
       <c r="Q69" s="25"/>
       <c r="R69"/>
     </row>
-    <row r="70" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="D70" s="1" t="b">
         <v>0</v>
@@ -3743,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>309</v>
+        <v>212</v>
       </c>
       <c r="G70" s="18"/>
       <c r="H70" s="15"/>
@@ -3758,24 +3802,24 @@
       <c r="Q70" s="25"/>
       <c r="R70"/>
     </row>
-    <row r="71" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>194</v>
+        <v>10</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
       <c r="D71" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E71" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>210</v>
+        <v>309</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="15"/>
@@ -3790,26 +3834,30 @@
       <c r="Q71" s="25"/>
       <c r="R71"/>
     </row>
-    <row r="72" spans="1:18" s="22" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="B72" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="D72" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E72" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F72" s="22" t="s">
-        <v>255</v>
+    <row r="72" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="G72" s="18"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
       <c r="L72" s="25"/>
       <c r="M72" s="38"/>
       <c r="N72" s="38"/>
@@ -3818,203 +3866,199 @@
       <c r="Q72" s="25"/>
       <c r="R72"/>
     </row>
-    <row r="73" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D73" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="1" t="b">
-        <v>0</v>
+    <row r="73" spans="1:18" s="22" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="D73" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="22" t="s">
+        <v>255</v>
       </c>
       <c r="G73" s="18"/>
-      <c r="H73" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="I73" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="J73" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="K73" s="38" t="s">
-        <v>307</v>
-      </c>
       <c r="L73" s="25"/>
-      <c r="M73" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="N73" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="O73" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="P73" s="38" t="s">
-        <v>310</v>
-      </c>
+      <c r="M73" s="38"/>
+      <c r="N73" s="38"/>
+      <c r="O73" s="38"/>
+      <c r="P73" s="38"/>
       <c r="Q73" s="25"/>
       <c r="R73"/>
     </row>
     <row r="74" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="B74" s="33" t="s">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="D74" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="33"/>
+      <c r="C74" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="G74" s="18"/>
-      <c r="H74" s="15"/>
-      <c r="I74" s="15"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
+      <c r="H74" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="I74" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="J74" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="K74" s="38" t="s">
+        <v>307</v>
+      </c>
       <c r="L74" s="25"/>
-      <c r="M74" s="38"/>
-      <c r="N74" s="38"/>
-      <c r="O74" s="38"/>
-      <c r="P74" s="38"/>
+      <c r="M74" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="N74" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="O74" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="P74" s="38" t="s">
+        <v>310</v>
+      </c>
       <c r="Q74" s="25"/>
       <c r="R74"/>
     </row>
-    <row r="75" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D75" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>16</v>
-      </c>
+    <row r="75" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A75" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B75" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="33" t="s">
+        <v>289</v>
+      </c>
+      <c r="D75" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" s="33"/>
       <c r="G75" s="18"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
       <c r="L75" s="25"/>
+      <c r="M75" s="38"/>
+      <c r="N75" s="38"/>
+      <c r="O75" s="38"/>
+      <c r="P75" s="38"/>
       <c r="Q75" s="25"/>
       <c r="R75"/>
     </row>
-    <row r="76" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="37" t="s">
-        <v>300</v>
-      </c>
-      <c r="B76" s="37" t="s">
-        <v>301</v>
-      </c>
-      <c r="C76" s="37" t="s">
-        <v>302</v>
-      </c>
-      <c r="D76" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F76" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="G76" s="25"/>
-      <c r="H76" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="I76" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="J76" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="K76" s="37" t="s">
-        <v>16</v>
-      </c>
+    <row r="76" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D76" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" s="18"/>
       <c r="L76" s="25"/>
-      <c r="M76" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N76" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O76" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P76" s="38" t="s">
-        <v>16</v>
-      </c>
       <c r="Q76" s="25"/>
       <c r="R76"/>
     </row>
-    <row r="77" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="18"/>
-      <c r="H77" s="15"/>
-      <c r="I77" s="15"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
+    <row r="77" spans="1:18" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A77" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="B77" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>302</v>
+      </c>
+      <c r="D77" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="25"/>
+      <c r="H77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J77" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="K77" s="37" t="s">
+        <v>16</v>
+      </c>
       <c r="L77" s="25"/>
-      <c r="M77" s="38"/>
-      <c r="N77" s="38"/>
-      <c r="O77" s="38"/>
-      <c r="P77" s="38"/>
+      <c r="M77" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N77" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="O77" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="P77" s="38" t="s">
+        <v>16</v>
+      </c>
       <c r="Q77" s="25"/>
       <c r="R77"/>
     </row>
     <row r="78" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="D78" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G78" s="18"/>
       <c r="H78" s="15"/>
@@ -4031,411 +4075,415 @@
     </row>
     <row r="79" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D79" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="F79" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G79" s="18"/>
-      <c r="H79" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="I79" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="J79" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="K79" s="38" t="s">
-        <v>307</v>
-      </c>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
       <c r="L79" s="25"/>
-      <c r="M79" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="N79" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="O79" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="P79" s="38" t="s">
-        <v>310</v>
-      </c>
+      <c r="M79" s="38"/>
+      <c r="N79" s="38"/>
+      <c r="O79" s="38"/>
+      <c r="P79" s="38"/>
       <c r="Q79" s="25"/>
       <c r="R79"/>
     </row>
     <row r="80" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D80" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="G80" s="18"/>
-      <c r="H80" s="15"/>
-      <c r="I80" s="15"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
+      <c r="H80" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="I80" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="J80" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="K80" s="38" t="s">
+        <v>307</v>
+      </c>
       <c r="L80" s="25"/>
-      <c r="M80" s="38"/>
-      <c r="N80" s="38"/>
-      <c r="O80" s="38"/>
-      <c r="P80" s="38"/>
+      <c r="M80" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="N80" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="O80" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="P80" s="38" t="s">
+        <v>310</v>
+      </c>
       <c r="Q80" s="25"/>
       <c r="R80"/>
     </row>
-    <row r="81" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D81" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>306</v>
+    <row r="81" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E81" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="G81" s="18"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
       <c r="L81" s="25"/>
+      <c r="M81" s="38"/>
+      <c r="N81" s="38"/>
+      <c r="O81" s="38"/>
+      <c r="P81" s="38"/>
       <c r="Q81" s="25"/>
       <c r="R81"/>
     </row>
-    <row r="82" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A82" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D82" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E82" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>19</v>
+    <row r="82" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D82" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" s="5" t="s">
+        <v>306</v>
       </c>
       <c r="G82" s="18"/>
-      <c r="H82" s="15"/>
-      <c r="I82" s="15"/>
-      <c r="J82" s="15"/>
-      <c r="K82" s="15"/>
       <c r="L82" s="25"/>
-      <c r="M82" s="38"/>
-      <c r="N82" s="38"/>
-      <c r="O82" s="38"/>
-      <c r="P82" s="38"/>
       <c r="Q82" s="25"/>
       <c r="R82"/>
     </row>
-    <row r="83" spans="1:19" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A83" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D83" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>213</v>
+    <row r="83" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A83" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G83" s="18"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
       <c r="L83" s="25"/>
+      <c r="M83" s="38"/>
+      <c r="N83" s="38"/>
+      <c r="O83" s="38"/>
+      <c r="P83" s="38"/>
       <c r="Q83" s="25"/>
       <c r="R83"/>
     </row>
-    <row r="84" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E84" s="1" t="b">
-        <v>0</v>
+    <row r="84" spans="1:19" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A84" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D84" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="G84" s="18"/>
-      <c r="H84" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="I84" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="J84" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="K84" s="15" t="s">
-        <v>308</v>
-      </c>
       <c r="L84" s="25"/>
-      <c r="M84" s="38" t="s">
-        <v>311</v>
-      </c>
-      <c r="N84" s="38" t="s">
-        <v>311</v>
-      </c>
-      <c r="O84" s="38" t="s">
-        <v>311</v>
-      </c>
-      <c r="P84" s="38" t="s">
-        <v>311</v>
-      </c>
       <c r="Q84" s="25"/>
       <c r="R84"/>
     </row>
     <row r="85" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E85" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="G85" s="18"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="15"/>
-      <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
+      <c r="H85" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="I85" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="J85" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="K85" s="15" t="s">
+        <v>308</v>
+      </c>
       <c r="L85" s="25"/>
-      <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
-      <c r="O85" s="38"/>
-      <c r="P85" s="38"/>
+      <c r="M85" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="N85" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="O85" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="P85" s="38" t="s">
+        <v>311</v>
+      </c>
       <c r="Q85" s="25"/>
       <c r="R85"/>
     </row>
-    <row r="86" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A86" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D86" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>93</v>
+    <row r="86" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D86" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="G86" s="18"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
       <c r="L86" s="25"/>
+      <c r="M86" s="38"/>
+      <c r="N86" s="38"/>
+      <c r="O86" s="38"/>
+      <c r="P86" s="38"/>
       <c r="Q86" s="25"/>
       <c r="R86"/>
     </row>
     <row r="87" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A87" s="5" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>5</v>
+        <v>94</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D87" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E87" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="G87" s="18"/>
       <c r="L87" s="25"/>
       <c r="Q87" s="25"/>
       <c r="R87"/>
     </row>
-    <row r="88" spans="1:19" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A88" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D88" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E88" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>97</v>
+    <row r="88" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D88" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G88" s="18"/>
-      <c r="H88" s="15"/>
-      <c r="I88" s="15"/>
-      <c r="J88" s="15"/>
-      <c r="K88" s="15"/>
       <c r="L88" s="25"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="38"/>
-      <c r="O88" s="38"/>
-      <c r="P88" s="38"/>
       <c r="Q88" s="25"/>
       <c r="R88"/>
     </row>
-    <row r="89" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:19" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B89" s="6"/>
-      <c r="C89" s="6"/>
+        <v>96</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D89" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E89" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="G89" s="18"/>
-      <c r="H89" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I89" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J89" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K89" s="15" t="s">
-        <v>4</v>
-      </c>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="15"/>
       <c r="L89" s="25"/>
-      <c r="M89" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N89" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O89" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P89" s="38" t="s">
-        <v>4</v>
-      </c>
+      <c r="M89" s="38"/>
+      <c r="N89" s="38"/>
+      <c r="O89" s="38"/>
+      <c r="P89" s="38"/>
       <c r="Q89" s="25"/>
       <c r="R89"/>
     </row>
     <row r="90" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
       <c r="D90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G90" s="18"/>
-      <c r="H90" s="15"/>
-      <c r="I90" s="15"/>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
+      <c r="H90" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I90" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J90" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K90" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="L90" s="25"/>
-      <c r="M90" s="38"/>
-      <c r="N90" s="38"/>
-      <c r="O90" s="38"/>
-      <c r="P90" s="38"/>
+      <c r="M90" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N90" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="O90" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="P90" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="Q90" s="25"/>
       <c r="R90"/>
     </row>
-    <row r="91" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B91" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C91" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="D91" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E91" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F91" s="28" t="s">
-        <v>269</v>
-      </c>
-      <c r="G91" s="25"/>
+    <row r="91" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D91" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E91" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G91" s="18"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="15"/>
       <c r="L91" s="25"/>
       <c r="M91" s="38"/>
       <c r="N91" s="38"/>
@@ -4444,30 +4492,26 @@
       <c r="Q91" s="25"/>
       <c r="R91"/>
     </row>
-    <row r="92" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A92" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="G92" s="18"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
+    <row r="92" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E92" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="G92" s="25"/>
       <c r="L92" s="25"/>
       <c r="M92" s="38"/>
       <c r="N92" s="38"/>
@@ -4476,24 +4520,24 @@
       <c r="Q92" s="25"/>
       <c r="R92"/>
     </row>
-    <row r="93" spans="1:19" s="12" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A93" s="12" t="s">
-        <v>248</v>
-      </c>
-      <c r="B93" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>250</v>
-      </c>
-      <c r="D93" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E93" s="12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>251</v>
+    <row r="93" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>252</v>
       </c>
       <c r="G93" s="18"/>
       <c r="H93" s="15"/>
@@ -4508,24 +4552,24 @@
       <c r="Q93" s="25"/>
       <c r="R93"/>
     </row>
-    <row r="94" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B94" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" t="s">
-        <v>278</v>
-      </c>
-      <c r="D94" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E94" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>25</v>
+    <row r="94" spans="1:19" s="12" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D94" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="G94" s="18"/>
       <c r="H94" s="15"/>
@@ -4540,72 +4584,72 @@
       <c r="Q94" s="25"/>
       <c r="R94"/>
     </row>
-    <row r="95" spans="1:19" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>276</v>
+    <row r="95" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="B95" t="s">
         <v>10</v>
       </c>
       <c r="C95" t="s">
-        <v>277</v>
-      </c>
-      <c r="D95" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" t="s">
+        <v>278</v>
+      </c>
+      <c r="D95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G95" s="25"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="15"/>
       <c r="L95" s="25"/>
+      <c r="M95" s="38"/>
+      <c r="N95" s="38"/>
+      <c r="O95" s="38"/>
+      <c r="P95" s="38"/>
       <c r="Q95" s="25"/>
       <c r="R95"/>
-      <c r="S95"/>
-    </row>
-    <row r="96" spans="1:19" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D96" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G96" s="18"/>
-      <c r="H96" s="15"/>
-      <c r="I96" s="15"/>
-      <c r="J96" s="15"/>
-      <c r="K96" s="15"/>
+    </row>
+    <row r="96" spans="1:19" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" t="s">
+        <v>277</v>
+      </c>
+      <c r="D96" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="25"/>
       <c r="L96" s="25"/>
-      <c r="M96" s="38"/>
-      <c r="N96" s="38"/>
-      <c r="O96" s="38"/>
-      <c r="P96" s="38"/>
       <c r="Q96" s="25"/>
       <c r="R96"/>
-    </row>
-    <row r="97" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="S96"/>
+    </row>
+    <row r="97" spans="1:19" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>56</v>
+        <v>5</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D97" s="1" t="b">
         <v>0</v>
@@ -4613,8 +4657,8 @@
       <c r="E97" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F97" s="4" t="s">
-        <v>214</v>
+      <c r="F97" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G97" s="18"/>
       <c r="H97" s="15"/>
@@ -4631,13 +4675,13 @@
     </row>
     <row r="98" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D98" s="1" t="b">
         <v>0</v>
@@ -4645,8 +4689,8 @@
       <c r="E98" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F98" s="1" t="s">
-        <v>16</v>
+      <c r="F98" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G98" s="18"/>
       <c r="H98" s="15"/>
@@ -4661,21 +4705,24 @@
       <c r="Q98" s="25"/>
       <c r="R98"/>
     </row>
-    <row r="99" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>205</v>
+        <v>105</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>206</v>
+        <v>106</v>
       </c>
       <c r="D99" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E99" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G99" s="18"/>
       <c r="H99" s="15"/>
@@ -4692,22 +4739,19 @@
     </row>
     <row r="100" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>107</v>
+        <v>205</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>110</v>
+        <v>206</v>
       </c>
       <c r="D100" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>108</v>
+        <v>1</v>
       </c>
       <c r="G100" s="18"/>
       <c r="H100" s="15"/>
@@ -4722,15 +4766,15 @@
       <c r="Q100" s="25"/>
       <c r="R100"/>
     </row>
-    <row r="101" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D101" s="1" t="b">
         <v>1</v>
@@ -4738,68 +4782,76 @@
       <c r="E101" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="F101" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="G101" s="18"/>
-      <c r="H101" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="I101" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="J101" s="38" t="s">
-        <v>307</v>
-      </c>
-      <c r="K101" s="38" t="s">
-        <v>307</v>
-      </c>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="15"/>
       <c r="L101" s="25"/>
-      <c r="M101" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="N101" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="O101" s="38" t="s">
-        <v>310</v>
-      </c>
-      <c r="P101" s="38" t="s">
-        <v>310</v>
-      </c>
+      <c r="M101" s="38"/>
+      <c r="N101" s="38"/>
+      <c r="O101" s="38"/>
+      <c r="P101" s="38"/>
       <c r="Q101" s="25"/>
       <c r="R101"/>
     </row>
-    <row r="102" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C102" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D102" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>220</v>
+    <row r="102" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D102" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G102" s="18"/>
+      <c r="H102" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="I102" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="J102" s="38" t="s">
+        <v>307</v>
+      </c>
+      <c r="K102" s="38" t="s">
+        <v>307</v>
+      </c>
       <c r="L102" s="25"/>
+      <c r="M102" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="N102" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="O102" s="38" t="s">
+        <v>310</v>
+      </c>
+      <c r="P102" s="38" t="s">
+        <v>310</v>
+      </c>
       <c r="Q102" s="25"/>
       <c r="R102"/>
     </row>
     <row r="103" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A103" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>67</v>
+        <v>12</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D103" s="5" t="b">
         <v>1</v>
@@ -4817,85 +4869,64 @@
     </row>
     <row r="104" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D104" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E104" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>16</v>
+        <v>220</v>
       </c>
       <c r="G104" s="18"/>
       <c r="L104" s="25"/>
       <c r="Q104" s="25"/>
       <c r="R104"/>
     </row>
-    <row r="105" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B105" s="1" t="s">
+    <row r="105" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A105" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D105" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E105" s="1" t="b">
-        <v>1</v>
+      <c r="C105" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D105" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E105" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G105" s="18"/>
-      <c r="H105" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I105" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J105" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K105" s="15" t="s">
-        <v>4</v>
-      </c>
       <c r="L105" s="25"/>
-      <c r="M105" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="N105" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O105" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P105" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="Q105" s="25"/>
       <c r="R105"/>
     </row>
     <row r="106" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D106" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="1" t="b">
         <v>1</v>
@@ -4931,23 +4962,23 @@
     </row>
     <row r="107" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D107" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="1" t="b">
         <v>1</v>
       </c>
       <c r="G107" s="18"/>
       <c r="H107" s="15" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I107" s="15" t="s">
         <v>4</v>
@@ -4960,7 +4991,7 @@
       </c>
       <c r="L107" s="25"/>
       <c r="M107" s="38" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="N107" s="38" t="s">
         <v>4</v>
@@ -4974,15 +5005,15 @@
       <c r="Q107" s="25"/>
       <c r="R107"/>
     </row>
-    <row r="108" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>0</v>
@@ -4990,133 +5021,133 @@
       <c r="E108" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="G108" s="18"/>
-      <c r="H108" s="15"/>
-      <c r="I108" s="15"/>
-      <c r="J108" s="15"/>
-      <c r="K108" s="15"/>
+      <c r="H108" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I108" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="L108" s="25"/>
-      <c r="M108" s="38"/>
-      <c r="N108" s="38"/>
-      <c r="O108" s="38"/>
-      <c r="P108" s="38"/>
+      <c r="M108" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N108" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O108" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="38" t="s">
+        <v>4</v>
+      </c>
       <c r="Q108" s="25"/>
       <c r="R108"/>
     </row>
-    <row r="109" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
+    <row r="109" spans="1:19" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A109" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D109" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G109" s="18"/>
+      <c r="H109" s="15"/>
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
+      <c r="K109" s="15"/>
+      <c r="L109" s="25"/>
+      <c r="M109" s="38"/>
+      <c r="N109" s="38"/>
+      <c r="O109" s="38"/>
+      <c r="P109" s="38"/>
+      <c r="Q109" s="25"/>
+      <c r="R109"/>
+    </row>
+    <row r="110" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
         <v>279</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B110" t="s">
         <v>5</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>280</v>
       </c>
-      <c r="D109" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
-        <v>4</v>
-      </c>
-      <c r="G109" s="25"/>
-      <c r="H109"/>
-      <c r="I109"/>
-      <c r="J109"/>
-      <c r="K109"/>
-      <c r="L109" s="21"/>
-      <c r="M109"/>
-      <c r="N109"/>
-      <c r="O109"/>
-      <c r="P109"/>
-      <c r="Q109" s="21"/>
-      <c r="R109"/>
-      <c r="S109"/>
-    </row>
-    <row r="110" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A110" s="5" t="s">
+      <c r="D110" t="b">
+        <v>0</v>
+      </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" t="s">
+        <v>4</v>
+      </c>
+      <c r="G110" s="25"/>
+      <c r="H110"/>
+      <c r="I110"/>
+      <c r="J110"/>
+      <c r="K110"/>
+      <c r="L110" s="21"/>
+      <c r="M110"/>
+      <c r="N110"/>
+      <c r="O110"/>
+      <c r="P110"/>
+      <c r="Q110" s="21"/>
+      <c r="R110"/>
+      <c r="S110"/>
+    </row>
+    <row r="111" spans="1:19" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A111" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B111" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C110" s="5" t="s">
+      <c r="C111" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D110" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E110" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F110" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G110" s="18"/>
-      <c r="L110" s="25"/>
-      <c r="Q110" s="25"/>
-      <c r="R110"/>
-    </row>
-    <row r="111" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D111" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" s="1" t="b">
-        <v>1</v>
+      <c r="D111" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="18"/>
-      <c r="H111" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I111" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J111" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K111" s="15" t="s">
-        <v>4</v>
-      </c>
       <c r="L111" s="25"/>
-      <c r="M111" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N111" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O111" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P111" s="38" t="s">
-        <v>4</v>
-      </c>
       <c r="Q111" s="25"/>
       <c r="R111"/>
     </row>
     <row r="112" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>240</v>
+        <v>128</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D112" s="1" t="b">
         <v>1</v>
@@ -5153,103 +5184,119 @@
       <c r="Q112" s="25"/>
       <c r="R112"/>
     </row>
-    <row r="113" spans="1:18" s="40" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A113" s="40" t="s">
+    <row r="113" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D113" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="18"/>
+      <c r="H113" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L113" s="25"/>
+      <c r="M113" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="N113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="O113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="25"/>
+      <c r="R113"/>
+    </row>
+    <row r="114" spans="1:18" s="40" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A114" s="40" t="s">
         <v>320</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B114" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C113" s="40" t="s">
+      <c r="C114" s="40" t="s">
         <v>321</v>
       </c>
-      <c r="D113" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E113" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="G113" s="25"/>
-      <c r="H113" s="40" t="s">
+      <c r="D114" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E114" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="G114" s="25"/>
+      <c r="H114" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="I113" s="40" t="s">
+      <c r="I114" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="J113" s="40" t="s">
+      <c r="J114" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="K113" s="40" t="s">
+      <c r="K114" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="L113" s="25"/>
-      <c r="M113" s="40" t="s">
+      <c r="L114" s="25"/>
+      <c r="M114" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="N113" s="40" t="s">
+      <c r="N114" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="O113" s="40" t="s">
+      <c r="O114" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="P113" s="40" t="s">
+      <c r="P114" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="Q113" s="25"/>
-    </row>
-    <row r="114" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A114" s="1" t="s">
+      <c r="Q114" s="25"/>
+    </row>
+    <row r="115" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A115" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B115" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C115" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D114" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E114" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F114" s="1" t="s">
+      <c r="D115" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G114" s="18"/>
-      <c r="H114" s="15"/>
-      <c r="I114" s="15"/>
-      <c r="J114" s="15"/>
-      <c r="K114" s="15"/>
-      <c r="L114" s="25"/>
-      <c r="M114" s="38"/>
-      <c r="N114" s="38"/>
-      <c r="O114" s="38"/>
-      <c r="P114" s="38"/>
-      <c r="Q114" s="25"/>
-      <c r="R114"/>
-    </row>
-    <row r="115" spans="1:18" s="23" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A115" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="B115" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="C115" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="D115" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F115" s="24" t="s">
-        <v>259</v>
-      </c>
-      <c r="G115" s="25"/>
-      <c r="H115" s="24"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="15"/>
+      <c r="J115" s="15"/>
+      <c r="K115" s="15"/>
       <c r="L115" s="25"/>
       <c r="M115" s="38"/>
       <c r="N115" s="38"/>
@@ -5258,30 +5305,27 @@
       <c r="Q115" s="25"/>
       <c r="R115"/>
     </row>
-    <row r="116" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A116" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D116" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="G116" s="18"/>
-      <c r="H116" s="15"/>
-      <c r="I116" s="15"/>
-      <c r="J116" s="15"/>
-      <c r="K116" s="15"/>
+    <row r="116" spans="1:18" s="23" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A116" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="B116" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C116" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="D116" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E116" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="G116" s="25"/>
+      <c r="H116" s="24"/>
       <c r="L116" s="25"/>
       <c r="M116" s="38"/>
       <c r="N116" s="38"/>
@@ -5289,6 +5333,38 @@
       <c r="P116" s="38"/>
       <c r="Q116" s="25"/>
       <c r="R116"/>
+    </row>
+    <row r="117" spans="1:18" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G117" s="18"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="25"/>
+      <c r="M117" s="38"/>
+      <c r="N117" s="38"/>
+      <c r="O117" s="38"/>
+      <c r="P117" s="38"/>
+      <c r="Q117" s="25"/>
+      <c r="R117"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
[EIGENAAR] correcties MIM11 config
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -1131,7 +1131,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1215,6 +1215,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1541,10 +1544,10 @@
   <dimension ref="A1:S117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L59" sqref="L59"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31:P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1763,16 +1766,16 @@
       <c r="R6"/>
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="43" t="b">
+      <c r="D7" s="44" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
@@ -1792,10 +1795,10 @@
       <c r="R7"/>
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
       <c r="G8" s="18"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
@@ -2581,29 +2584,29 @@
       </c>
       <c r="G31" s="25"/>
       <c r="H31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="I31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="J31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="K31" s="38" t="s">
-        <v>306</v>
+        <v>25</v>
+      </c>
+      <c r="I31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="43" t="s">
+        <v>25</v>
       </c>
       <c r="L31" s="25"/>
-      <c r="M31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="N31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="O31" s="38" t="s">
-        <v>306</v>
-      </c>
-      <c r="P31" s="38" t="s">
-        <v>306</v>
+      <c r="M31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="N31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="O31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="P31" s="43" t="s">
+        <v>25</v>
       </c>
       <c r="Q31" s="25"/>
       <c r="R31"/>
@@ -2912,27 +2915,27 @@
       <c r="H40" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K40" s="15" t="s">
-        <v>4</v>
+      <c r="I40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="43" t="s">
+        <v>16</v>
       </c>
       <c r="L40" s="25"/>
-      <c r="M40" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O40" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P40" s="38" t="s">
-        <v>4</v>
+      <c r="M40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="N40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="P40" s="43" t="s">
+        <v>16</v>
       </c>
       <c r="Q40" s="25"/>
       <c r="R40"/>
@@ -3063,16 +3066,16 @@
       <c r="R44"/>
     </row>
     <row r="45" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="43" t="s">
+      <c r="A45" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="B45" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="43" t="b">
+      <c r="D45" s="44" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="b">
@@ -3095,10 +3098,10 @@
       <c r="R45"/>
     </row>
     <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="43"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="A46" s="44"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
       <c r="G46" s="18"/>
       <c r="H46" s="15"/>
       <c r="I46" s="15"/>

</xml_diff>

<commit_message>
Correctie Json defaults EIGENAAR.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA3278-0936-449B-8ACD-486837408F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12060"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EIGENAAR" sheetId="3" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="330">
   <si>
     <t>Name</t>
   </si>
@@ -1012,12 +1013,15 @@
   </si>
   <si>
     <t>NEN3610_GML322</t>
+  </si>
+  <si>
+    <t>kadaster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1143,7 +1147,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1165,22 +1169,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1196,30 +1188,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1232,50 +1200,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
-    <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
-    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Controlecel" xfId="1" builtinId="23"/>
+    <cellStyle name="Goed" xfId="4" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Verklarende tekst" xfId="3" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1552,17 +1484,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A77" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1573,19 +1505,19 @@
     <col min="4" max="4" width="13.23046875" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="5.4609375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="5.4609375" style="17" customWidth="1"/>
     <col min="8" max="8" width="16.15234375" customWidth="1"/>
     <col min="9" max="9" width="16.07421875" customWidth="1"/>
     <col min="10" max="10" width="15.69140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.765625" customWidth="1"/>
     <col min="12" max="12" width="16.07421875" customWidth="1"/>
-    <col min="13" max="13" width="4.4609375" style="21" customWidth="1"/>
+    <col min="13" max="13" width="4.4609375" style="17" customWidth="1"/>
     <col min="14" max="14" width="16.15234375" customWidth="1"/>
     <col min="15" max="15" width="16.07421875" customWidth="1"/>
     <col min="16" max="16" width="15.69140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.765625" customWidth="1"/>
     <col min="18" max="18" width="16.07421875" customWidth="1"/>
-    <col min="19" max="19" width="4.4609375" style="21" customWidth="1"/>
+    <col min="19" max="19" width="4.4609375" style="17" customWidth="1"/>
     <col min="20" max="20" width="27.3046875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1608,7 +1540,7 @@
       <c r="F1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G1" s="16"/>
+      <c r="G1" s="12"/>
       <c r="H1" s="3" t="s">
         <v>253</v>
       </c>
@@ -1624,7 +1556,7 @@
       <c r="L1" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="M1" s="16"/>
+      <c r="M1" s="12"/>
       <c r="N1" s="3" t="s">
         <v>253</v>
       </c>
@@ -1640,12 +1572,12 @@
       <c r="R1" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="16"/>
+      <c r="S1" s="12"/>
       <c r="T1"/>
     </row>
     <row r="2" spans="1:20" s="3" customFormat="1" ht="37.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" s="2"/>
-      <c r="G2" s="17"/>
+      <c r="G2" s="13"/>
       <c r="H2" s="2" t="s">
         <v>311</v>
       </c>
@@ -1661,7 +1593,7 @@
       <c r="L2" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="M2" s="17"/>
+      <c r="M2" s="13"/>
       <c r="N2" s="2" t="s">
         <v>315</v>
       </c>
@@ -1677,7 +1609,7 @@
       <c r="R2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="S2" s="17"/>
+      <c r="S2" s="13"/>
       <c r="T2"/>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="44.15" thickTop="1" x14ac:dyDescent="0.4">
@@ -1696,19 +1628,9 @@
       <c r="E3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="25"/>
+      <c r="G3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="S3" s="14"/>
       <c r="T3"/>
     </row>
     <row r="4" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1730,19 +1652,9 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="25"/>
+      <c r="G4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="S4" s="14"/>
       <c r="T4"/>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -1764,19 +1676,9 @@
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="25"/>
+      <c r="G5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="S5" s="14"/>
       <c r="T5"/>
     </row>
     <row r="6" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -1795,60 +1697,40 @@
       <c r="E6" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="M6" s="25"/>
-      <c r="S6" s="25"/>
+      <c r="G6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="S6" s="14"/>
       <c r="T6"/>
     </row>
     <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="45" t="b">
+      <c r="D7" s="21" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="44"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="25"/>
+      <c r="G7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="S7" s="14"/>
       <c r="T7"/>
     </row>
     <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="44"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="25"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="G8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="S8" s="14"/>
       <c r="T8"/>
     </row>
     <row r="9" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -1870,9 +1752,9 @@
       <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="M9" s="25"/>
-      <c r="S9" s="25"/>
+      <c r="G9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="S9" s="14"/>
       <c r="T9"/>
     </row>
     <row r="10" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1894,19 +1776,9 @@
       <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="25"/>
+      <c r="G10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="S10" s="14"/>
       <c r="T10"/>
     </row>
     <row r="11" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1925,9 +1797,9 @@
       <c r="E11" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G11" s="18"/>
-      <c r="M11" s="25"/>
-      <c r="S11" s="25"/>
+      <c r="G11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="S11" s="14"/>
       <c r="T11"/>
     </row>
     <row r="12" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -1949,53 +1821,33 @@
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="44"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="38"/>
-      <c r="O12" s="38"/>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="44"/>
-      <c r="S12" s="25"/>
+      <c r="G12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="S12" s="14"/>
       <c r="T12"/>
     </row>
-    <row r="13" spans="1:20" s="11" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D13" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="25"/>
+      <c r="G13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="S13" s="14"/>
       <c r="T13"/>
     </row>
     <row r="14" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2017,19 +1869,9 @@
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="25"/>
+      <c r="G14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="S14" s="14"/>
       <c r="T14"/>
     </row>
     <row r="15" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2048,39 +1890,39 @@
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L15" s="44" t="s">
+      <c r="L15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="25"/>
-      <c r="N15" s="38" t="s">
+      <c r="M15" s="14"/>
+      <c r="N15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O15" s="38" t="s">
+      <c r="O15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="P15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="Q15" s="38" t="s">
+      <c r="Q15" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="R15" s="44" t="s">
+      <c r="R15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="S15" s="25"/>
+      <c r="S15" s="14"/>
       <c r="T15"/>
     </row>
     <row r="16" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2102,19 +1944,9 @@
       <c r="F16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="38"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="38"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="25"/>
+      <c r="G16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="S16" s="14"/>
       <c r="T16"/>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2136,19 +1968,9 @@
       <c r="F17" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="38"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="25"/>
+      <c r="G17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="S17" s="14"/>
       <c r="T17"/>
     </row>
     <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2166,19 +1988,9 @@
       <c r="F18" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="38"/>
-      <c r="O18" s="38"/>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="38"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="25"/>
+      <c r="G18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="S18" s="14"/>
       <c r="T18"/>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2197,19 +2009,9 @@
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="25"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="25"/>
+      <c r="G19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="S19" s="14"/>
       <c r="T19"/>
     </row>
     <row r="20" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2228,22 +2030,12 @@
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="32" t="s">
+      <c r="F20" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="25"/>
-      <c r="N20" s="38"/>
-      <c r="O20" s="38"/>
-      <c r="P20" s="38"/>
-      <c r="Q20" s="38"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="25"/>
+      <c r="G20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="S20" s="14"/>
       <c r="T20"/>
     </row>
     <row r="21" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2262,22 +2054,12 @@
       <c r="E21" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="38"/>
-      <c r="O21" s="38"/>
-      <c r="P21" s="38"/>
-      <c r="Q21" s="38"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="25"/>
+      <c r="G21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="S21" s="14"/>
       <c r="T21"/>
     </row>
     <row r="22" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2296,39 +2078,39 @@
       <c r="E22" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L22" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M22" s="25"/>
-      <c r="N22" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q22" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R22" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S22" s="25"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="14"/>
+      <c r="N22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S22" s="14"/>
       <c r="T22"/>
     </row>
     <row r="23" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2350,9 +2132,9 @@
       <c r="F23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="M23" s="25"/>
-      <c r="S23" s="25"/>
+      <c r="G23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="S23" s="14"/>
       <c r="T23"/>
     </row>
     <row r="24" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2371,19 +2153,9 @@
       <c r="E24" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="38"/>
-      <c r="O24" s="38"/>
-      <c r="P24" s="38"/>
-      <c r="Q24" s="38"/>
-      <c r="R24" s="44"/>
-      <c r="S24" s="25"/>
+      <c r="G24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="S24" s="14"/>
       <c r="T24"/>
     </row>
     <row r="25" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -2402,39 +2174,39 @@
       <c r="E25" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L25" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="25"/>
-      <c r="N25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P25" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q25" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R25" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S25" s="25"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M25" s="14"/>
+      <c r="N25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S25" s="14"/>
       <c r="T25"/>
     </row>
     <row r="26" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2453,69 +2225,63 @@
       <c r="E26" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K26" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P26" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q26" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R26" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S26" s="25"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="14"/>
+      <c r="N26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S26" s="14"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" s="36" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A27" s="36" t="s">
+    <row r="27" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D27" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G27" s="25"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="38"/>
-      <c r="R27" s="44"/>
-      <c r="S27" s="25"/>
+      <c r="D27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="S27" s="14"/>
       <c r="T27"/>
     </row>
     <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2534,39 +2300,39 @@
       <c r="E28" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M28" s="25"/>
-      <c r="N28" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R28" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S28" s="25"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28" s="14"/>
+      <c r="N28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S28" s="14"/>
       <c r="T28"/>
     </row>
     <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2585,141 +2351,87 @@
       <c r="E29" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M29" s="25"/>
-      <c r="N29" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q29" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R29" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S29" s="25"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" s="14"/>
+      <c r="N29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S29" s="14"/>
       <c r="T29"/>
     </row>
-    <row r="30" spans="1:20" s="26" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D30" s="26" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="26" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" s="25"/>
-      <c r="H30" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="I30" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="L30" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="25"/>
-      <c r="N30" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O30" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q30" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R30" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S30" s="25"/>
+      <c r="D30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="S30" s="14"/>
       <c r="T30"/>
     </row>
-    <row r="31" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D31" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="K31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="L31" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="M31" s="25"/>
-      <c r="N31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="O31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="P31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q31" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="R31" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="S31" s="25"/>
+      <c r="D31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="S31" s="14"/>
       <c r="T31"/>
     </row>
     <row r="32" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2741,19 +2453,9 @@
       <c r="F32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="18"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="38"/>
-      <c r="O32" s="38"/>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="38"/>
-      <c r="R32" s="44"/>
-      <c r="S32" s="25"/>
+      <c r="G32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="S32" s="14"/>
       <c r="T32"/>
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -2772,19 +2474,9 @@
       <c r="E33" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="44"/>
-      <c r="S33" s="25"/>
+      <c r="G33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="S33" s="14"/>
       <c r="T33"/>
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2803,73 +2495,63 @@
       <c r="E34" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G34" s="18"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="38"/>
-      <c r="O34" s="38"/>
-      <c r="P34" s="38"/>
-      <c r="Q34" s="38"/>
-      <c r="R34" s="44"/>
-      <c r="S34" s="25"/>
+      <c r="G34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="S34" s="14"/>
       <c r="T34"/>
     </row>
-    <row r="35" spans="1:20" s="29" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A35" s="29" t="s">
+    <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B35" s="29" t="s">
+      <c r="B35" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D35" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="29" t="s">
+      <c r="D35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="G35" s="25"/>
-      <c r="H35" s="29" t="s">
+      <c r="G35" s="14"/>
+      <c r="H35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I35" s="29" t="s">
+      <c r="I35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="J35" s="29" t="s">
+      <c r="J35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="K35" s="29" t="s">
+      <c r="K35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="L35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="M35" s="25"/>
-      <c r="N35" s="41" t="s">
+      <c r="M35" s="14"/>
+      <c r="N35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="O35" s="41" t="s">
+      <c r="O35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="P35" s="41" t="s">
+      <c r="P35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="Q35" s="41" t="s">
+      <c r="Q35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="R35" s="44" t="s">
+      <c r="R35" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="S35" s="25"/>
+      <c r="S35" s="14"/>
       <c r="T35"/>
     </row>
     <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -2888,63 +2570,63 @@
       <c r="E36" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L36" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" s="25"/>
-      <c r="N36" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P36" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R36" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S36" s="25"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" s="14"/>
+      <c r="N36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S36" s="14"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="30" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="30" t="s">
+    <row r="37" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="D37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="31"/>
-      <c r="M37" s="25"/>
-      <c r="S37" s="25"/>
+      <c r="D37" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="19"/>
+      <c r="M37" s="14"/>
+      <c r="S37" s="14"/>
       <c r="T37"/>
     </row>
     <row r="38" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -2963,39 +2645,39 @@
       <c r="E38" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G38" s="18"/>
-      <c r="H38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L38" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="25"/>
-      <c r="N38" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P38" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q38" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R38" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S38" s="25"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="14"/>
+      <c r="N38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S38" s="14"/>
       <c r="T38"/>
     </row>
     <row r="39" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3017,19 +2699,9 @@
       <c r="F39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="18"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
-      <c r="K39" s="15"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="38"/>
-      <c r="O39" s="38"/>
-      <c r="P39" s="38"/>
-      <c r="Q39" s="38"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="25"/>
+      <c r="G39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="S39" s="14"/>
       <c r="T39"/>
     </row>
     <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3048,90 +2720,90 @@
       <c r="E40" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="J40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="L40" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" s="25"/>
-      <c r="N40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="O40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="P40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q40" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="R40" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S40" s="25"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" s="14"/>
+      <c r="N40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S40" s="14"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="27" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="27" t="s">
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D41" s="27" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="27" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="25"/>
-      <c r="H41" s="27" t="s">
+      <c r="D41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="I41" s="28" t="s">
+      <c r="I41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J41" s="28" t="s">
+      <c r="J41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="K41" s="28" t="s">
+      <c r="K41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="L41" s="44" t="s">
+      <c r="L41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="M41" s="25"/>
-      <c r="N41" s="38" t="s">
+      <c r="M41" s="14"/>
+      <c r="N41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="O41" s="38" t="s">
+      <c r="O41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="P41" s="38" t="s">
+      <c r="P41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="Q41" s="38" t="s">
+      <c r="Q41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="R41" s="44" t="s">
+      <c r="R41" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="S41" s="25"/>
+      <c r="S41" s="14"/>
       <c r="T41"/>
     </row>
     <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3153,19 +2825,9 @@
       <c r="F42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
-      <c r="J42" s="15"/>
-      <c r="K42" s="15"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="38"/>
-      <c r="O42" s="38"/>
-      <c r="P42" s="38"/>
-      <c r="Q42" s="38"/>
-      <c r="R42" s="44"/>
-      <c r="S42" s="25"/>
+      <c r="G42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="S42" s="14"/>
       <c r="T42"/>
     </row>
     <row r="43" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3187,9 +2849,9 @@
       <c r="F43" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G43" s="18"/>
-      <c r="M43" s="25"/>
-      <c r="S43" s="25"/>
+      <c r="G43" s="14"/>
+      <c r="M43" s="14"/>
+      <c r="S43" s="14"/>
       <c r="T43"/>
     </row>
     <row r="44" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3211,22 +2873,22 @@
       <c r="F44" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G44" s="18"/>
-      <c r="M44" s="25"/>
-      <c r="S44" s="25"/>
+      <c r="G44" s="14"/>
+      <c r="M44" s="14"/>
+      <c r="S44" s="14"/>
       <c r="T44"/>
     </row>
     <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="45" t="s">
+      <c r="A45" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="45" t="s">
+      <c r="B45" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="D45" s="45" t="b">
+      <c r="D45" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="b">
@@ -3235,39 +2897,19 @@
       <c r="F45" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
-      <c r="J45" s="15"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="38"/>
-      <c r="P45" s="38"/>
-      <c r="Q45" s="38"/>
-      <c r="R45" s="44"/>
-      <c r="S45" s="25"/>
+      <c r="G45" s="14"/>
+      <c r="M45" s="14"/>
+      <c r="S45" s="14"/>
       <c r="T45"/>
     </row>
     <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="45"/>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45"/>
-      <c r="D46" s="45"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="44"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="38"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="38"/>
-      <c r="R46" s="44"/>
-      <c r="S46" s="25"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="G46" s="14"/>
+      <c r="M46" s="14"/>
+      <c r="S46" s="14"/>
       <c r="T46"/>
     </row>
     <row r="47" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3286,19 +2928,9 @@
       <c r="E47" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G47" s="18"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="44"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="38"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="38"/>
-      <c r="R47" s="44"/>
-      <c r="S47" s="25"/>
+      <c r="G47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="S47" s="14"/>
       <c r="T47"/>
     </row>
     <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3320,19 +2952,9 @@
       <c r="F48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="18"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="44"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="38"/>
-      <c r="O48" s="38"/>
-      <c r="P48" s="38"/>
-      <c r="Q48" s="38"/>
-      <c r="R48" s="44"/>
-      <c r="S48" s="25"/>
+      <c r="G48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="S48" s="14"/>
       <c r="T48"/>
     </row>
     <row r="49" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3354,19 +2976,9 @@
       <c r="F49" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
-      <c r="J49" s="15"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="44"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="38"/>
-      <c r="O49" s="38"/>
-      <c r="P49" s="38"/>
-      <c r="Q49" s="38"/>
-      <c r="R49" s="44"/>
-      <c r="S49" s="25"/>
+      <c r="G49" s="15"/>
+      <c r="M49" s="14"/>
+      <c r="S49" s="14"/>
       <c r="T49"/>
     </row>
     <row r="50" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3381,39 +2993,39 @@
       <c r="E50" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G50" s="19"/>
-      <c r="H50" s="38" t="s">
+      <c r="G50" s="15"/>
+      <c r="H50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I50" s="38" t="s">
+      <c r="I50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J50" s="38" t="s">
+      <c r="J50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K50" s="38" t="s">
+      <c r="K50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L50" s="44" t="s">
+      <c r="L50" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M50" s="19"/>
-      <c r="N50" s="38" t="s">
+      <c r="M50" s="15"/>
+      <c r="N50" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O50" s="38" t="s">
+      <c r="O50" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P50" s="38" t="s">
+      <c r="P50" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q50" s="38" t="s">
+      <c r="Q50" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R50" s="44" t="s">
+      <c r="R50" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="S50" s="19"/>
+      <c r="S50" s="15"/>
       <c r="T50"/>
     </row>
     <row r="51" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3435,9 +3047,9 @@
       <c r="F51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="18"/>
-      <c r="M51" s="25"/>
-      <c r="S51" s="25"/>
+      <c r="G51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="S51" s="14"/>
       <c r="T51"/>
     </row>
     <row r="52" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3459,9 +3071,9 @@
       <c r="F52" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G52" s="18"/>
-      <c r="M52" s="25"/>
-      <c r="S52" s="25"/>
+      <c r="G52" s="14"/>
+      <c r="M52" s="14"/>
+      <c r="S52" s="14"/>
       <c r="T52"/>
     </row>
     <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3483,19 +3095,9 @@
       <c r="F53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G53" s="18"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="44"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="38"/>
-      <c r="O53" s="38"/>
-      <c r="P53" s="38"/>
-      <c r="Q53" s="38"/>
-      <c r="R53" s="44"/>
-      <c r="S53" s="25"/>
+      <c r="G53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="S53" s="14"/>
       <c r="T53"/>
     </row>
     <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3517,19 +3119,9 @@
       <c r="F54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G54" s="18"/>
-      <c r="H54" s="15"/>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="44"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="38"/>
-      <c r="O54" s="38"/>
-      <c r="P54" s="38"/>
-      <c r="Q54" s="38"/>
-      <c r="R54" s="44"/>
-      <c r="S54" s="25"/>
+      <c r="G54" s="14"/>
+      <c r="M54" s="14"/>
+      <c r="S54" s="14"/>
       <c r="T54"/>
     </row>
     <row r="55" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3551,9 +3143,9 @@
       <c r="F55" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G55" s="18"/>
-      <c r="M55" s="25"/>
-      <c r="S55" s="25"/>
+      <c r="G55" s="14"/>
+      <c r="M55" s="14"/>
+      <c r="S55" s="14"/>
       <c r="T55"/>
     </row>
     <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3575,98 +3167,88 @@
       <c r="F56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="15"/>
-      <c r="J56" s="15"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="44"/>
-      <c r="M56" s="25"/>
-      <c r="N56" s="38"/>
-      <c r="O56" s="38"/>
-      <c r="P56" s="38"/>
-      <c r="Q56" s="38"/>
-      <c r="R56" s="44"/>
-      <c r="S56" s="25"/>
+      <c r="G56" s="14"/>
+      <c r="M56" s="14"/>
+      <c r="S56" s="14"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="42" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="42" t="s">
+    <row r="57" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B57" s="42" t="s">
+      <c r="B57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="42" t="s">
+      <c r="C57" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="42" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="25"/>
-      <c r="I57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="K57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="L57" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M57" s="25"/>
-      <c r="O57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="P57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q57" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="R57" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S57" s="25"/>
+      <c r="D57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="I57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M57" s="14"/>
+      <c r="O57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S57" s="14"/>
     </row>
     <row r="58" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="D58" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="14"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="L58" s="14"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="14"/>
-      <c r="Q58" s="14"/>
-      <c r="R58" s="14"/>
-      <c r="S58" s="20"/>
+      <c r="D58" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="16"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="11"/>
+      <c r="S58" s="16"/>
     </row>
     <row r="59" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="5" t="s">
@@ -3687,9 +3269,9 @@
       <c r="F59" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="G59" s="25"/>
-      <c r="M59" s="25"/>
-      <c r="S59" s="25"/>
+      <c r="G59" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="S59" s="14"/>
       <c r="T59"/>
     </row>
     <row r="60" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3708,20 +3290,20 @@
       <c r="E60" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F60" s="32"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-      <c r="M60" s="25"/>
-      <c r="N60" s="32"/>
-      <c r="O60" s="32"/>
-      <c r="P60" s="32"/>
-      <c r="Q60" s="32"/>
-      <c r="R60" s="32"/>
-      <c r="S60" s="25"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="20"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="20"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="14"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
+      <c r="S60" s="14"/>
       <c r="T60"/>
     </row>
     <row r="61" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3740,9 +3322,9 @@
       <c r="E61" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G61" s="25"/>
-      <c r="M61" s="25"/>
-      <c r="S61" s="25"/>
+      <c r="G61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="S61" s="14"/>
       <c r="T61"/>
     </row>
     <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3764,9 +3346,9 @@
       <c r="F62" t="s">
         <v>303</v>
       </c>
-      <c r="G62" s="25"/>
-      <c r="M62" s="25"/>
-      <c r="S62" s="25"/>
+      <c r="G62" s="14"/>
+      <c r="M62" s="14"/>
+      <c r="S62" s="14"/>
       <c r="T62"/>
     </row>
     <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3788,43 +3370,43 @@
       <c r="F63" t="s">
         <v>299</v>
       </c>
-      <c r="G63" s="25"/>
-      <c r="M63" s="25"/>
-      <c r="S63" s="25"/>
+      <c r="G63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="S63" s="14"/>
       <c r="T63"/>
     </row>
     <row r="64" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="11" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="C64" s="13" t="s">
+      <c r="C64" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="D64" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="14" t="s">
+      <c r="D64" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="11" t="s">
         <v>292</v>
       </c>
-      <c r="G64" s="20"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
-      <c r="L64" s="14"/>
-      <c r="M64" s="20"/>
-      <c r="N64" s="14"/>
-      <c r="O64" s="14"/>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-      <c r="S64" s="20"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="16"/>
     </row>
     <row r="65" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
@@ -3845,9 +3427,9 @@
       <c r="F65" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G65" s="18"/>
-      <c r="M65" s="25"/>
-      <c r="S65" s="25"/>
+      <c r="G65" s="14"/>
+      <c r="M65" s="14"/>
+      <c r="S65" s="14"/>
       <c r="T65"/>
     </row>
     <row r="66" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -3869,49 +3451,33 @@
       <c r="F66" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G66" s="18"/>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="44"/>
-      <c r="M66" s="25"/>
-      <c r="N66" s="38"/>
-      <c r="O66" s="38"/>
-      <c r="P66" s="38"/>
-      <c r="Q66" s="38"/>
-      <c r="R66" s="44"/>
-      <c r="S66" s="25"/>
+      <c r="G66" s="14"/>
+      <c r="M66" s="14"/>
+      <c r="S66" s="14"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" s="34" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>290</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
       </c>
-      <c r="C67" s="13" t="s">
+      <c r="C67" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="D67" s="34" t="b">
+      <c r="D67" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E67" t="b">
         <v>1</v>
       </c>
-      <c r="F67" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="G67" s="25"/>
-      <c r="L67" s="44"/>
-      <c r="M67" s="25"/>
-      <c r="N67" s="38"/>
-      <c r="O67" s="38"/>
-      <c r="P67" s="38"/>
-      <c r="Q67" s="38"/>
-      <c r="R67" s="44"/>
-      <c r="S67" s="25"/>
+      <c r="F67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="S67" s="14"/>
       <c r="T67"/>
     </row>
     <row r="68" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3933,9 +3499,9 @@
       <c r="F68" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G68" s="18"/>
-      <c r="M68" s="25"/>
-      <c r="S68" s="25"/>
+      <c r="G68" s="14"/>
+      <c r="M68" s="14"/>
+      <c r="S68" s="14"/>
       <c r="T68"/>
     </row>
     <row r="69" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -3957,9 +3523,9 @@
       <c r="F69" t="s">
         <v>228</v>
       </c>
-      <c r="G69" s="25"/>
-      <c r="M69" s="25"/>
-      <c r="S69" s="25"/>
+      <c r="G69" s="14"/>
+      <c r="M69" s="14"/>
+      <c r="S69" s="14"/>
       <c r="T69"/>
     </row>
     <row r="70" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -3981,19 +3547,9 @@
       <c r="F70" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G70" s="18"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="44"/>
-      <c r="M70" s="25"/>
-      <c r="N70" s="38"/>
-      <c r="O70" s="38"/>
-      <c r="P70" s="38"/>
-      <c r="Q70" s="38"/>
-      <c r="R70" s="44"/>
-      <c r="S70" s="25"/>
+      <c r="G70" s="14"/>
+      <c r="M70" s="14"/>
+      <c r="S70" s="14"/>
       <c r="T70"/>
     </row>
     <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4015,19 +3571,9 @@
       <c r="F71" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="G71" s="18"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="15"/>
-      <c r="L71" s="44"/>
-      <c r="M71" s="25"/>
-      <c r="N71" s="38"/>
-      <c r="O71" s="38"/>
-      <c r="P71" s="38"/>
-      <c r="Q71" s="38"/>
-      <c r="R71" s="44"/>
-      <c r="S71" s="25"/>
+      <c r="G71" s="14"/>
+      <c r="M71" s="14"/>
+      <c r="S71" s="14"/>
       <c r="T71"/>
     </row>
     <row r="72" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4049,49 +3595,33 @@
       <c r="F72" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="G72" s="18"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="44"/>
-      <c r="M72" s="25"/>
-      <c r="N72" s="38"/>
-      <c r="O72" s="38"/>
-      <c r="P72" s="38"/>
-      <c r="Q72" s="38"/>
-      <c r="R72" s="44"/>
-      <c r="S72" s="25"/>
+      <c r="G72" s="14"/>
+      <c r="M72" s="14"/>
+      <c r="S72" s="14"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="22" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A73" s="22" t="s">
+    <row r="73" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="22" t="s">
+      <c r="C73" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D73" s="22" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="22" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" s="22" t="s">
+      <c r="D73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G73" s="18"/>
-      <c r="L73" s="44"/>
-      <c r="M73" s="25"/>
-      <c r="N73" s="38"/>
-      <c r="O73" s="38"/>
-      <c r="P73" s="38"/>
-      <c r="Q73" s="38"/>
-      <c r="R73" s="44"/>
-      <c r="S73" s="25"/>
+      <c r="G73" s="14"/>
+      <c r="M73" s="14"/>
+      <c r="S73" s="14"/>
       <c r="T73"/>
     </row>
     <row r="74" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4110,71 +3640,60 @@
       <c r="E74" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G74" s="18"/>
-      <c r="H74" s="38" t="s">
+      <c r="G74" s="14"/>
+      <c r="H74" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I74" s="38" t="s">
+      <c r="I74" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J74" s="38" t="s">
+      <c r="J74" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K74" s="38" t="s">
+      <c r="K74" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L74" s="44" t="s">
+      <c r="L74" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M74" s="25"/>
-      <c r="N74" s="38" t="s">
+      <c r="M74" s="14"/>
+      <c r="N74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O74" s="38" t="s">
+      <c r="O74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P74" s="38" t="s">
+      <c r="P74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q74" s="38" t="s">
+      <c r="Q74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R74" s="44" t="s">
+      <c r="R74" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="S74" s="25"/>
+      <c r="S74" s="14"/>
       <c r="T74"/>
     </row>
     <row r="75" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B75" s="33" t="s">
+      <c r="B75" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="33" t="s">
+      <c r="C75" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D75" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="F75" s="33"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="15"/>
-      <c r="I75" s="15"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="44"/>
-      <c r="M75" s="25"/>
-      <c r="N75" s="38"/>
-      <c r="O75" s="38"/>
-      <c r="P75" s="38"/>
-      <c r="Q75" s="38"/>
-      <c r="R75" s="44"/>
-      <c r="S75" s="25"/>
+      <c r="D75" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G75" s="14"/>
+      <c r="M75" s="14"/>
+      <c r="S75" s="14"/>
       <c r="T75"/>
     </row>
     <row r="76" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -4196,43 +3715,43 @@
       <c r="F76" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G76" s="18"/>
-      <c r="M76" s="25"/>
-      <c r="S76" s="25"/>
+      <c r="G76" s="14"/>
+      <c r="M76" s="14"/>
+      <c r="S76" s="14"/>
       <c r="T76"/>
     </row>
     <row r="77" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A77" s="37" t="s">
+      <c r="A77" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B77" s="37" t="s">
+      <c r="B77" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C77" s="37" t="s">
+      <c r="C77" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D77" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E77" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="F77" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="G77" s="25"/>
-      <c r="H77" s="37"/>
-      <c r="I77" s="37"/>
-      <c r="J77" s="37"/>
-      <c r="K77" s="37"/>
-      <c r="L77" s="44"/>
-      <c r="M77" s="25"/>
-      <c r="N77" s="38"/>
-      <c r="O77" s="38"/>
-      <c r="P77" s="38"/>
-      <c r="Q77" s="38"/>
-      <c r="R77" s="44"/>
-      <c r="S77" s="25"/>
+      <c r="D77" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" s="14"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="14"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="14"/>
       <c r="T77"/>
     </row>
     <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4254,19 +3773,9 @@
       <c r="F78" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G78" s="18"/>
-      <c r="H78" s="15"/>
-      <c r="I78" s="15"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="44"/>
-      <c r="M78" s="25"/>
-      <c r="N78" s="38"/>
-      <c r="O78" s="38"/>
-      <c r="P78" s="38"/>
-      <c r="Q78" s="38"/>
-      <c r="R78" s="44"/>
-      <c r="S78" s="25"/>
+      <c r="G78" s="14"/>
+      <c r="M78" s="14"/>
+      <c r="S78" s="14"/>
       <c r="T78"/>
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4288,19 +3797,9 @@
       <c r="F79" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G79" s="18"/>
-      <c r="H79" s="15"/>
-      <c r="I79" s="15"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="44"/>
-      <c r="M79" s="25"/>
-      <c r="N79" s="38"/>
-      <c r="O79" s="38"/>
-      <c r="P79" s="38"/>
-      <c r="Q79" s="38"/>
-      <c r="R79" s="44"/>
-      <c r="S79" s="25"/>
+      <c r="G79" s="14"/>
+      <c r="M79" s="14"/>
+      <c r="S79" s="14"/>
       <c r="T79"/>
     </row>
     <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4319,39 +3818,39 @@
       <c r="E80" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G80" s="18"/>
-      <c r="H80" s="38" t="s">
+      <c r="G80" s="14"/>
+      <c r="H80" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I80" s="38" t="s">
+      <c r="I80" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J80" s="38" t="s">
+      <c r="J80" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K80" s="38" t="s">
+      <c r="K80" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L80" s="44" t="s">
+      <c r="L80" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M80" s="25"/>
-      <c r="N80" s="38" t="s">
+      <c r="M80" s="14"/>
+      <c r="N80" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O80" s="38" t="s">
+      <c r="O80" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P80" s="38" t="s">
+      <c r="P80" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q80" s="38" t="s">
+      <c r="Q80" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R80" s="44" t="s">
+      <c r="R80" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="S80" s="25"/>
+      <c r="S80" s="14"/>
       <c r="T80"/>
     </row>
     <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4373,19 +3872,9 @@
       <c r="F81" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G81" s="18"/>
-      <c r="H81" s="15"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="44"/>
-      <c r="M81" s="25"/>
-      <c r="N81" s="38"/>
-      <c r="O81" s="38"/>
-      <c r="P81" s="38"/>
-      <c r="Q81" s="38"/>
-      <c r="R81" s="44"/>
-      <c r="S81" s="25"/>
+      <c r="G81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="S81" s="14"/>
       <c r="T81"/>
     </row>
     <row r="82" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -4407,9 +3896,9 @@
       <c r="F82" s="5" t="s">
         <v>306</v>
       </c>
-      <c r="G82" s="18"/>
-      <c r="M82" s="25"/>
-      <c r="S82" s="25"/>
+      <c r="G82" s="14"/>
+      <c r="M82" s="14"/>
+      <c r="S82" s="14"/>
       <c r="T82"/>
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4431,19 +3920,9 @@
       <c r="F83" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G83" s="18"/>
-      <c r="H83" s="15"/>
-      <c r="I83" s="15"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="44"/>
-      <c r="M83" s="25"/>
-      <c r="N83" s="38"/>
-      <c r="O83" s="38"/>
-      <c r="P83" s="38"/>
-      <c r="Q83" s="38"/>
-      <c r="R83" s="44"/>
-      <c r="S83" s="25"/>
+      <c r="G83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="S83" s="14"/>
       <c r="T83"/>
     </row>
     <row r="84" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
@@ -4465,9 +3944,9 @@
       <c r="F84" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="G84" s="18"/>
-      <c r="M84" s="25"/>
-      <c r="S84" s="25"/>
+      <c r="G84" s="14"/>
+      <c r="M84" s="14"/>
+      <c r="S84" s="14"/>
       <c r="T84"/>
     </row>
     <row r="85" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4486,39 +3965,39 @@
       <c r="E85" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G85" s="18"/>
-      <c r="H85" s="15" t="s">
+      <c r="G85" s="14"/>
+      <c r="H85" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I85" s="15" t="s">
+      <c r="I85" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="J85" s="15" t="s">
+      <c r="J85" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="K85" s="15" t="s">
+      <c r="K85" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="L85" s="44" t="s">
+      <c r="L85" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="M85" s="25"/>
-      <c r="N85" s="38" t="s">
+      <c r="M85" s="14"/>
+      <c r="N85" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="O85" s="38" t="s">
+      <c r="O85" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="P85" s="38" t="s">
+      <c r="P85" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="Q85" s="38" t="s">
+      <c r="Q85" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="R85" s="44" t="s">
+      <c r="R85" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="S85" s="25"/>
+      <c r="S85" s="14"/>
       <c r="T85"/>
     </row>
     <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4540,19 +4019,9 @@
       <c r="F86" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G86" s="18"/>
-      <c r="H86" s="15"/>
-      <c r="I86" s="15"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
-      <c r="L86" s="44"/>
-      <c r="M86" s="25"/>
-      <c r="N86" s="38"/>
-      <c r="O86" s="38"/>
-      <c r="P86" s="38"/>
-      <c r="Q86" s="38"/>
-      <c r="R86" s="44"/>
-      <c r="S86" s="25"/>
+      <c r="G86" s="14"/>
+      <c r="M86" s="14"/>
+      <c r="S86" s="14"/>
       <c r="T86"/>
     </row>
     <row r="87" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4574,9 +4043,9 @@
       <c r="F87" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="G87" s="18"/>
-      <c r="M87" s="25"/>
-      <c r="S87" s="25"/>
+      <c r="G87" s="14"/>
+      <c r="M87" s="14"/>
+      <c r="S87" s="14"/>
       <c r="T87"/>
     </row>
     <row r="88" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4598,47 +4067,47 @@
       <c r="F88" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G88" s="18"/>
-      <c r="M88" s="25"/>
-      <c r="S88" s="25"/>
+      <c r="G88" s="14"/>
+      <c r="M88" s="14"/>
+      <c r="S88" s="14"/>
       <c r="T88"/>
     </row>
     <row r="89" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="30" t="s">
+      <c r="A89" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="30" t="s">
+      <c r="C89" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="D89" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="G89" s="25"/>
-      <c r="H89" s="30"/>
-      <c r="I89" s="30"/>
-      <c r="J89" s="30"/>
-      <c r="K89" s="30"/>
-      <c r="L89" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="M89" s="31"/>
-      <c r="N89" s="30"/>
-      <c r="O89" s="30"/>
-      <c r="P89" s="30"/>
-      <c r="Q89" s="30"/>
-      <c r="R89" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="S89" s="25"/>
+      <c r="D89" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" s="14"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M89" s="19"/>
+      <c r="N89" s="18"/>
+      <c r="O89" s="18"/>
+      <c r="P89" s="18"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="S89" s="14"/>
       <c r="T89"/>
     </row>
     <row r="90" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
@@ -4660,19 +4129,9 @@
       <c r="F90" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G90" s="18"/>
-      <c r="H90" s="15"/>
-      <c r="I90" s="15"/>
-      <c r="J90" s="15"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="44"/>
-      <c r="M90" s="25"/>
-      <c r="N90" s="38"/>
-      <c r="O90" s="38"/>
-      <c r="P90" s="38"/>
-      <c r="Q90" s="38"/>
-      <c r="R90" s="44"/>
-      <c r="S90" s="25"/>
+      <c r="G90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="S90" s="14"/>
       <c r="T90"/>
     </row>
     <row r="91" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4687,39 +4146,39 @@
       <c r="E91" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G91" s="18"/>
-      <c r="H91" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K91" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L91" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="M91" s="25"/>
-      <c r="N91" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O91" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="P91" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q91" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R91" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="S91" s="25"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M91" s="14"/>
+      <c r="N91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q91" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S91" s="14"/>
       <c r="T91"/>
     </row>
     <row r="92" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4741,49 +4200,33 @@
       <c r="F92" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G92" s="18"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="15"/>
-      <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
-      <c r="L92" s="44"/>
-      <c r="M92" s="25"/>
-      <c r="N92" s="38"/>
-      <c r="O92" s="38"/>
-      <c r="P92" s="38"/>
-      <c r="Q92" s="38"/>
-      <c r="R92" s="44"/>
-      <c r="S92" s="25"/>
+      <c r="G92" s="14"/>
+      <c r="M92" s="14"/>
+      <c r="S92" s="14"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="28" t="s">
+    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B93" s="28" t="s">
+      <c r="B93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="28" t="s">
+      <c r="C93" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D93" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="28" t="s">
+      <c r="D93" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="G93" s="25"/>
-      <c r="L93" s="44"/>
-      <c r="M93" s="25"/>
-      <c r="N93" s="38"/>
-      <c r="O93" s="38"/>
-      <c r="P93" s="38"/>
-      <c r="Q93" s="38"/>
-      <c r="R93" s="44"/>
-      <c r="S93" s="25"/>
+      <c r="G93" s="14"/>
+      <c r="M93" s="14"/>
+      <c r="S93" s="14"/>
       <c r="T93"/>
     </row>
     <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4802,56 +4245,36 @@
       <c r="E94" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F94" s="10" t="s">
+      <c r="F94" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="G94" s="18"/>
-      <c r="H94" s="15"/>
-      <c r="I94" s="15"/>
-      <c r="J94" s="15"/>
-      <c r="K94" s="15"/>
-      <c r="L94" s="44"/>
-      <c r="M94" s="25"/>
-      <c r="N94" s="38"/>
-      <c r="O94" s="38"/>
-      <c r="P94" s="38"/>
-      <c r="Q94" s="38"/>
-      <c r="R94" s="44"/>
-      <c r="S94" s="25"/>
+      <c r="G94" s="14"/>
+      <c r="M94" s="14"/>
+      <c r="S94" s="14"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A95" s="12" t="s">
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C95" s="12" t="s">
+      <c r="C95" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="D95" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E95" s="12" t="b">
+      <c r="D95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F95" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="G95" s="18"/>
-      <c r="H95" s="15"/>
-      <c r="I95" s="15"/>
-      <c r="J95" s="15"/>
-      <c r="K95" s="15"/>
-      <c r="L95" s="44"/>
-      <c r="M95" s="25"/>
-      <c r="N95" s="38"/>
-      <c r="O95" s="38"/>
-      <c r="P95" s="38"/>
-      <c r="Q95" s="38"/>
-      <c r="R95" s="44"/>
-      <c r="S95" s="25"/>
+      <c r="G95" s="14"/>
+      <c r="M95" s="14"/>
+      <c r="S95" s="14"/>
       <c r="T95"/>
     </row>
     <row r="96" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -4873,19 +4296,9 @@
       <c r="F96" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G96" s="18"/>
-      <c r="H96" s="15"/>
-      <c r="I96" s="15"/>
-      <c r="J96" s="15"/>
-      <c r="K96" s="15"/>
-      <c r="L96" s="44"/>
-      <c r="M96" s="25"/>
-      <c r="N96" s="38"/>
-      <c r="O96" s="38"/>
-      <c r="P96" s="38"/>
-      <c r="Q96" s="38"/>
-      <c r="R96" s="44"/>
-      <c r="S96" s="25"/>
+      <c r="G96" s="14"/>
+      <c r="M96" s="14"/>
+      <c r="S96" s="14"/>
       <c r="T96"/>
     </row>
     <row r="97" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -4907,9 +4320,9 @@
       <c r="F97" t="s">
         <v>25</v>
       </c>
-      <c r="G97" s="25"/>
-      <c r="M97" s="25"/>
-      <c r="S97" s="25"/>
+      <c r="G97" s="14"/>
+      <c r="M97" s="14"/>
+      <c r="S97" s="14"/>
       <c r="T97"/>
       <c r="U97"/>
     </row>
@@ -4932,19 +4345,9 @@
       <c r="F98" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G98" s="18"/>
-      <c r="H98" s="15"/>
-      <c r="I98" s="15"/>
-      <c r="J98" s="15"/>
-      <c r="K98" s="15"/>
-      <c r="L98" s="44"/>
-      <c r="M98" s="25"/>
-      <c r="N98" s="38"/>
-      <c r="O98" s="38"/>
-      <c r="P98" s="38"/>
-      <c r="Q98" s="38"/>
-      <c r="R98" s="44"/>
-      <c r="S98" s="25"/>
+      <c r="G98" s="14"/>
+      <c r="M98" s="14"/>
+      <c r="S98" s="14"/>
       <c r="T98"/>
     </row>
     <row r="99" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -4966,19 +4369,9 @@
       <c r="F99" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="G99" s="18"/>
-      <c r="H99" s="15"/>
-      <c r="I99" s="15"/>
-      <c r="J99" s="15"/>
-      <c r="K99" s="15"/>
-      <c r="L99" s="44"/>
-      <c r="M99" s="25"/>
-      <c r="N99" s="38"/>
-      <c r="O99" s="38"/>
-      <c r="P99" s="38"/>
-      <c r="Q99" s="38"/>
-      <c r="R99" s="44"/>
-      <c r="S99" s="25"/>
+      <c r="G99" s="14"/>
+      <c r="M99" s="14"/>
+      <c r="S99" s="14"/>
       <c r="T99"/>
     </row>
     <row r="100" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -5000,19 +4393,9 @@
       <c r="F100" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G100" s="18"/>
-      <c r="H100" s="15"/>
-      <c r="I100" s="15"/>
-      <c r="J100" s="15"/>
-      <c r="K100" s="15"/>
-      <c r="L100" s="44"/>
-      <c r="M100" s="25"/>
-      <c r="N100" s="38"/>
-      <c r="O100" s="38"/>
-      <c r="P100" s="38"/>
-      <c r="Q100" s="38"/>
-      <c r="R100" s="44"/>
-      <c r="S100" s="25"/>
+      <c r="G100" s="14"/>
+      <c r="M100" s="14"/>
+      <c r="S100" s="14"/>
       <c r="T100"/>
     </row>
     <row r="101" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5031,19 +4414,9 @@
       <c r="E101" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G101" s="18"/>
-      <c r="H101" s="15"/>
-      <c r="I101" s="15"/>
-      <c r="J101" s="15"/>
-      <c r="K101" s="15"/>
-      <c r="L101" s="44"/>
-      <c r="M101" s="25"/>
-      <c r="N101" s="38"/>
-      <c r="O101" s="38"/>
-      <c r="P101" s="38"/>
-      <c r="Q101" s="38"/>
-      <c r="R101" s="44"/>
-      <c r="S101" s="25"/>
+      <c r="G101" s="14"/>
+      <c r="M101" s="14"/>
+      <c r="S101" s="14"/>
       <c r="T101"/>
     </row>
     <row r="102" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5065,19 +4438,9 @@
       <c r="F102" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G102" s="18"/>
-      <c r="H102" s="15"/>
-      <c r="I102" s="15"/>
-      <c r="J102" s="15"/>
-      <c r="K102" s="15"/>
-      <c r="L102" s="44"/>
-      <c r="M102" s="25"/>
-      <c r="N102" s="38"/>
-      <c r="O102" s="38"/>
-      <c r="P102" s="38"/>
-      <c r="Q102" s="38"/>
-      <c r="R102" s="44"/>
-      <c r="S102" s="25"/>
+      <c r="G102" s="14"/>
+      <c r="M102" s="14"/>
+      <c r="S102" s="14"/>
       <c r="T102"/>
     </row>
     <row r="103" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -5096,39 +4459,39 @@
       <c r="E103" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G103" s="18"/>
-      <c r="H103" s="38" t="s">
+      <c r="G103" s="14"/>
+      <c r="H103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I103" s="38" t="s">
+      <c r="I103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J103" s="38" t="s">
+      <c r="J103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K103" s="38" t="s">
+      <c r="K103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L103" s="44" t="s">
+      <c r="L103" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M103" s="25"/>
-      <c r="N103" s="38" t="s">
+      <c r="M103" s="14"/>
+      <c r="N103" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O103" s="38" t="s">
+      <c r="O103" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P103" s="38" t="s">
+      <c r="P103" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q103" s="38" t="s">
+      <c r="Q103" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R103" s="44" t="s">
+      <c r="R103" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="S103" s="25"/>
+      <c r="S103" s="14"/>
       <c r="T103"/>
     </row>
     <row r="104" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -5150,9 +4513,9 @@
       <c r="F104" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G104" s="18"/>
-      <c r="M104" s="25"/>
-      <c r="S104" s="25"/>
+      <c r="G104" s="14"/>
+      <c r="M104" s="14"/>
+      <c r="S104" s="14"/>
       <c r="T104"/>
     </row>
     <row r="105" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -5174,9 +4537,9 @@
       <c r="F105" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="G105" s="18"/>
-      <c r="M105" s="25"/>
-      <c r="S105" s="25"/>
+      <c r="G105" s="14"/>
+      <c r="M105" s="14"/>
+      <c r="S105" s="14"/>
       <c r="T105"/>
     </row>
     <row r="106" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -5198,9 +4561,9 @@
       <c r="F106" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G106" s="18"/>
-      <c r="M106" s="25"/>
-      <c r="S106" s="25"/>
+      <c r="G106" s="14"/>
+      <c r="M106" s="14"/>
+      <c r="S106" s="14"/>
       <c r="T106"/>
     </row>
     <row r="107" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5219,39 +4582,39 @@
       <c r="E107" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G107" s="18"/>
-      <c r="H107" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I107" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M107" s="25"/>
-      <c r="N107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R107" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S107" s="25"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M107" s="14"/>
+      <c r="N107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S107" s="14"/>
       <c r="T107"/>
     </row>
     <row r="108" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5270,39 +4633,39 @@
       <c r="E108" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G108" s="18"/>
-      <c r="H108" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I108" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J108" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K108" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L108" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M108" s="25"/>
-      <c r="N108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="O108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q108" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R108" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S108" s="25"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M108" s="14"/>
+      <c r="N108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S108" s="14"/>
       <c r="T108"/>
     </row>
     <row r="109" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5321,39 +4684,39 @@
       <c r="E109" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G109" s="18"/>
-      <c r="H109" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M109" s="25"/>
-      <c r="N109" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O109" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R109" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S109" s="25"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M109" s="14"/>
+      <c r="N109" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S109" s="14"/>
       <c r="T109"/>
     </row>
     <row r="110" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -5375,19 +4738,9 @@
       <c r="F110" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G110" s="18"/>
-      <c r="H110" s="15"/>
-      <c r="I110" s="15"/>
-      <c r="J110" s="15"/>
-      <c r="K110" s="15"/>
-      <c r="L110" s="44"/>
-      <c r="M110" s="25"/>
-      <c r="N110" s="38"/>
-      <c r="O110" s="38"/>
-      <c r="P110" s="38"/>
-      <c r="Q110" s="38"/>
-      <c r="R110" s="44"/>
-      <c r="S110" s="25"/>
+      <c r="G110" s="14"/>
+      <c r="M110" s="14"/>
+      <c r="S110" s="14"/>
       <c r="T110"/>
     </row>
     <row r="111" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
@@ -5409,19 +4762,19 @@
       <c r="F111" t="s">
         <v>4</v>
       </c>
-      <c r="G111" s="25"/>
+      <c r="G111" s="14"/>
       <c r="H111"/>
       <c r="I111"/>
       <c r="J111"/>
       <c r="K111"/>
       <c r="L111"/>
-      <c r="M111" s="21"/>
+      <c r="M111" s="17"/>
       <c r="N111"/>
       <c r="O111"/>
       <c r="P111"/>
       <c r="Q111"/>
       <c r="R111"/>
-      <c r="S111" s="21"/>
+      <c r="S111" s="17"/>
       <c r="T111"/>
       <c r="U111"/>
     </row>
@@ -5444,9 +4797,9 @@
       <c r="F112" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G112" s="18"/>
-      <c r="M112" s="25"/>
-      <c r="S112" s="25"/>
+      <c r="G112" s="14"/>
+      <c r="M112" s="14"/>
+      <c r="S112" s="14"/>
       <c r="T112"/>
     </row>
     <row r="113" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5465,39 +4818,39 @@
       <c r="E113" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G113" s="18"/>
-      <c r="H113" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I113" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J113" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K113" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L113" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M113" s="25"/>
-      <c r="N113" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O113" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P113" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q113" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R113" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S113" s="25"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M113" s="14"/>
+      <c r="N113" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S113" s="14"/>
       <c r="T113"/>
     </row>
     <row r="114" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
@@ -5516,90 +4869,90 @@
       <c r="E114" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G114" s="18"/>
-      <c r="H114" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I114" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="J114" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K114" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="L114" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M114" s="25"/>
-      <c r="N114" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="O114" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="P114" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q114" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="R114" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="S114" s="25"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M114" s="14"/>
+      <c r="N114" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S114" s="14"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:20" s="40" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A115" s="40" t="s">
+    <row r="115" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A115" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C115" s="40" t="s">
+      <c r="C115" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="D115" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E115" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="25"/>
-      <c r="H115" s="40" t="s">
+      <c r="D115" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E115" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" s="14"/>
+      <c r="H115" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="I115" s="40" t="s">
+      <c r="I115" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="J115" s="40" t="s">
+      <c r="J115" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K115" s="40" t="s">
+      <c r="K115" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="L115" s="44" t="s">
+      <c r="L115" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="M115" s="25"/>
-      <c r="N115" s="40" t="s">
+      <c r="M115" s="14"/>
+      <c r="N115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="O115" s="40" t="s">
+      <c r="O115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="P115" s="40" t="s">
+      <c r="P115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="Q115" s="40" t="s">
+      <c r="Q115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="R115" s="44" t="s">
+      <c r="R115" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="S115" s="25"/>
+      <c r="S115" s="14"/>
     </row>
     <row r="116" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
@@ -5620,50 +4973,33 @@
       <c r="F116" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G116" s="18"/>
-      <c r="H116" s="15"/>
-      <c r="I116" s="15"/>
-      <c r="J116" s="15"/>
-      <c r="K116" s="15"/>
-      <c r="L116" s="44"/>
-      <c r="M116" s="25"/>
-      <c r="N116" s="38"/>
-      <c r="O116" s="38"/>
-      <c r="P116" s="38"/>
-      <c r="Q116" s="38"/>
-      <c r="R116" s="44"/>
-      <c r="S116" s="25"/>
+      <c r="G116" s="14"/>
+      <c r="M116" s="14"/>
+      <c r="S116" s="14"/>
       <c r="T116"/>
     </row>
-    <row r="117" spans="1:20" s="23" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A117" s="24" t="s">
+    <row r="117" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A117" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B117" s="24" t="s">
+      <c r="B117" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C117" s="24" t="s">
+      <c r="C117" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="D117" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="24" t="s">
+      <c r="D117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F117" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="G117" s="25"/>
-      <c r="H117" s="24"/>
-      <c r="L117" s="44"/>
-      <c r="M117" s="25"/>
-      <c r="N117" s="38"/>
-      <c r="O117" s="38"/>
-      <c r="P117" s="38"/>
-      <c r="Q117" s="38"/>
-      <c r="R117" s="44"/>
-      <c r="S117" s="25"/>
+      <c r="G117" s="14"/>
+      <c r="M117" s="14"/>
+      <c r="S117" s="14"/>
       <c r="T117"/>
     </row>
     <row r="118" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
@@ -5685,19 +5021,9 @@
       <c r="F118" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G118" s="18"/>
-      <c r="H118" s="15"/>
-      <c r="I118" s="15"/>
-      <c r="J118" s="15"/>
-      <c r="K118" s="15"/>
-      <c r="L118" s="44"/>
-      <c r="M118" s="25"/>
-      <c r="N118" s="38"/>
-      <c r="O118" s="38"/>
-      <c r="P118" s="38"/>
-      <c r="Q118" s="38"/>
-      <c r="R118" s="44"/>
-      <c r="S118" s="25"/>
+      <c r="G118" s="14"/>
+      <c r="M118" s="14"/>
+      <c r="S118" s="14"/>
       <c r="T118"/>
     </row>
   </sheetData>
@@ -5712,8 +5038,8 @@
     <mergeCell ref="D45:D46"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
-    <hyperlink ref="F21" r:id="rId2"/>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="37" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -5721,7 +5047,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Uitbreiding eigenaar sample owner
Standaard mopdulen voor conceptuele modellen: msword, respec, skos,
mimformat.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AA3278-0936-449B-8ACD-486837408F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50250C7-8178-4D99-B82A-98899994578D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="345">
   <si>
     <t>Name</t>
   </si>
@@ -1016,6 +1016,51 @@
   </si>
   <si>
     <t>kadaster</t>
+  </si>
+  <si>
+    <t>createeatoolbox</t>
+  </si>
+  <si>
+    <t>Should an EA toolbox be generated?</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>createmimformat</t>
+  </si>
+  <si>
+    <t>Yes if MIM format must be generated</t>
+  </si>
+  <si>
+    <t>xml|rdf-xml|turtle|legacy</t>
+  </si>
+  <si>
+    <t>The type of the MIM format file generated</t>
+  </si>
+  <si>
+    <t>mimformatname</t>
+  </si>
+  <si>
+    <t>The name of the MIM format file generated</t>
+  </si>
+  <si>
+    <t>mimformattype</t>
+  </si>
+  <si>
+    <t>xml</t>
+  </si>
+  <si>
+    <t>mimformatversion</t>
+  </si>
+  <si>
+    <t>v1|v2</t>
+  </si>
+  <si>
+    <t>The version of the MIM compiler</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -1488,13 +1533,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U118"/>
+  <dimension ref="A1:U123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2260,15 +2305,15 @@
       <c r="S26" s="14"/>
       <c r="T26"/>
     </row>
-    <row r="27" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>293</v>
+        <v>330</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>294</v>
+        <v>331</v>
       </c>
       <c r="D27" s="1" t="b">
         <v>0</v>
@@ -2276,77 +2321,76 @@
       <c r="E27" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G27" s="14"/>
+      <c r="H27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M27" s="14"/>
+      <c r="N27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S27" s="14"/>
-      <c r="T27"/>
-    </row>
-    <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="28" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>293</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>33</v>
+        <v>294</v>
       </c>
       <c r="D28" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F28" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G28" s="14"/>
-      <c r="H28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M28" s="14"/>
-      <c r="N28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R28" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S28" s="14"/>
       <c r="T28"/>
     </row>
     <row r="29" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>146</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1" t="b">
         <v>1</v>
@@ -2356,7 +2400,7 @@
         <v>16</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>4</v>
@@ -2365,14 +2409,14 @@
         <v>4</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="M29" s="14"/>
       <c r="N29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>4</v>
@@ -2381,20 +2425,20 @@
         <v>4</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="S29" s="14"/>
       <c r="T29"/>
     </row>
     <row r="30" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>260</v>
+        <v>146</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>261</v>
+        <v>147</v>
       </c>
       <c r="D30" s="1" t="b">
         <v>0</v>
@@ -2402,23 +2446,50 @@
       <c r="E30" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G30" s="14"/>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M30" s="14"/>
+      <c r="N30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S30" s="14"/>
       <c r="T30"/>
     </row>
     <row r="31" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
@@ -2427,22 +2498,22 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>329</v>
+        <v>16</v>
       </c>
       <c r="G31" s="14"/>
       <c r="M31" s="14"/>
       <c r="S31" s="14"/>
       <c r="T31"/>
     </row>
-    <row r="32" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>265</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>266</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>0</v>
@@ -2451,22 +2522,22 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>35</v>
+        <v>329</v>
       </c>
       <c r="G32" s="14"/>
       <c r="M32" s="14"/>
       <c r="S32" s="14"/>
       <c r="T32"/>
     </row>
-    <row r="33" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>170</v>
+        <v>333</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>172</v>
+        <v>334</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
@@ -2474,26 +2545,46 @@
       <c r="E33" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G33" s="14"/>
+      <c r="I33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M33" s="14"/>
+      <c r="R33" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S33" s="14"/>
-      <c r="T33"/>
-    </row>
-    <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="34" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>173</v>
+        <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>174</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>175</v>
+        <v>37</v>
       </c>
       <c r="D34" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E34" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="G34" s="14"/>
       <c r="M34" s="14"/>
@@ -2502,13 +2593,13 @@
     </row>
     <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>270</v>
+        <v>170</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>271</v>
+        <v>171</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>272</v>
+        <v>172</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>0</v>
@@ -2516,53 +2607,20 @@
       <c r="E35" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="G35" s="14"/>
-      <c r="H35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="M35" s="14"/>
-      <c r="N35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>321</v>
-      </c>
       <c r="S35" s="14"/>
       <c r="T35"/>
     </row>
     <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>39</v>
+        <v>175</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>0</v>
@@ -2570,74 +2628,77 @@
       <c r="E36" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="G36" s="14"/>
-      <c r="H36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M36" s="14"/>
-      <c r="N36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S36" s="14"/>
       <c r="T36"/>
     </row>
-    <row r="37" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>275</v>
-      </c>
-      <c r="D37" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G37" s="19"/>
+    <row r="37" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="M37" s="14"/>
+      <c r="N37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="S37" s="14"/>
       <c r="T37"/>
     </row>
-    <row r="38" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38" s="1" t="b">
         <v>0</v>
@@ -2680,39 +2741,51 @@
       <c r="S38" s="14"/>
       <c r="T38"/>
     </row>
-    <row r="39" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="1" t="s">
+    <row r="39" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G39" s="14"/>
+      <c r="C39" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="I39" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L39" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="M39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D40" s="1" t="b">
         <v>0</v>
@@ -2728,10 +2801,10 @@
         <v>16</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>16</v>
@@ -2744,10 +2817,10 @@
         <v>16</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="R40" s="1" t="s">
         <v>16</v>
@@ -2755,66 +2828,39 @@
       <c r="S40" s="14"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
-        <v>264</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>267</v>
+        <v>43</v>
       </c>
       <c r="D41" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G41" s="14"/>
-      <c r="H41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="L41" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="M41" s="14"/>
-      <c r="N41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>268</v>
-      </c>
       <c r="S41" s="14"/>
       <c r="T41"/>
     </row>
     <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>176</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="D42" s="1" t="b">
         <v>0</v>
@@ -2822,79 +2868,133 @@
       <c r="E42" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G42" s="14"/>
+      <c r="H42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M42" s="14"/>
+      <c r="N42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S42" s="14"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>16</v>
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G43" s="14"/>
+      <c r="H43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="M43" s="14"/>
+      <c r="N43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="S43" s="14"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>220</v>
+    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G44" s="14"/>
       <c r="M44" s="14"/>
       <c r="S44" s="14"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="21" t="s">
+    <row r="45" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="C45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="14"/>
@@ -2902,31 +3002,48 @@
       <c r="S45" s="14"/>
       <c r="T45"/>
     </row>
-    <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
+    <row r="46" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>220</v>
+      </c>
       <c r="G46" s="14"/>
       <c r="M46" s="14"/>
       <c r="S46" s="14"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A47" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D47" s="1" t="b">
+    <row r="47" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G47" s="14"/>
       <c r="M47" s="14"/>
@@ -2934,24 +3051,10 @@
       <c r="T47"/>
     </row>
     <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
       <c r="G48" s="14"/>
       <c r="M48" s="14"/>
       <c r="S48" s="14"/>
@@ -2959,188 +3062,185 @@
     </row>
     <row r="49" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
-        <v>55</v>
+        <v>178</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>179</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="D49" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G49" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="G49" s="14"/>
       <c r="M49" s="14"/>
       <c r="S49" s="14"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D50" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G50" s="15"/>
-      <c r="H50" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="L50" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="M50" s="15"/>
-      <c r="N50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R50" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="S50" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="M50" s="14"/>
+      <c r="S50" s="14"/>
       <c r="T50"/>
     </row>
-    <row r="51" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D51" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G51" s="14"/>
+    <row r="51" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G51" s="15"/>
       <c r="M51" s="14"/>
       <c r="S51" s="14"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A52" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D52" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="S52" s="14"/>
+    <row r="52" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" s="15"/>
+      <c r="H52" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="M52" s="15"/>
+      <c r="N52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="S52" s="15"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="1" t="s">
+    <row r="53" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>16</v>
+      <c r="C53" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="G53" s="14"/>
       <c r="M53" s="14"/>
       <c r="S53" s="14"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>16</v>
+    <row r="54" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D54" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="G54" s="14"/>
       <c r="M54" s="14"/>
       <c r="S54" s="14"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55" s="5" t="s">
+    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D55" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="5" t="s">
+      <c r="C55" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G55" s="14"/>
@@ -3150,13 +3250,13 @@
     </row>
     <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
-        <v>186</v>
+        <v>60</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>187</v>
+        <v>61</v>
       </c>
       <c r="D56" s="1" t="b">
         <v>0</v>
@@ -3172,155 +3272,150 @@
       <c r="S56" s="14"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" s="14"/>
+      <c r="M57" s="14"/>
+      <c r="S57" s="14"/>
+      <c r="T57"/>
+    </row>
+    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" s="14"/>
+      <c r="M58" s="14"/>
+      <c r="S58" s="14"/>
+      <c r="T58"/>
+    </row>
+    <row r="59" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A59" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="D57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G57" s="14"/>
-      <c r="I57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M57" s="14"/>
-      <c r="O57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S57" s="14"/>
-    </row>
-    <row r="58" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A58" s="11" t="s">
+      <c r="D59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" s="14"/>
+      <c r="I59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M59" s="14"/>
+      <c r="O59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S59" s="14"/>
+    </row>
+    <row r="60" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A60" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B60" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C60" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="D58" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="16"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="16"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="11"/>
-      <c r="S58" s="16"/>
-    </row>
-    <row r="59" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="5" t="s">
+      <c r="D60" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="11"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="16"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="11"/>
+      <c r="S60" s="16"/>
+    </row>
+    <row r="61" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B61" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="D59" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F59" s="5" t="s">
+      <c r="D61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="G59" s="14"/>
-      <c r="M59" s="14"/>
-      <c r="S59" s="14"/>
-      <c r="T59"/>
-    </row>
-    <row r="60" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="20"/>
-      <c r="L60" s="20"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="20"/>
-      <c r="O60" s="20"/>
-      <c r="P60" s="20"/>
-      <c r="Q60" s="20"/>
-      <c r="R60" s="20"/>
-      <c r="S60" s="14"/>
-      <c r="T60"/>
-    </row>
-    <row r="61" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A61" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D61" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="5" t="b">
-        <v>1</v>
       </c>
       <c r="G61" s="14"/>
       <c r="M61" s="14"/>
@@ -3328,248 +3423,253 @@
       <c r="T61"/>
     </row>
     <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>295</v>
-      </c>
-      <c r="B62" t="s">
-        <v>82</v>
-      </c>
-      <c r="C62" t="s">
-        <v>297</v>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" t="s">
-        <v>303</v>
-      </c>
+      <c r="A62" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="D62" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="20"/>
       <c r="G62" s="14"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="20"/>
+      <c r="L62" s="20"/>
       <c r="M62" s="14"/>
+      <c r="N62" s="20"/>
+      <c r="O62" s="20"/>
+      <c r="P62" s="20"/>
+      <c r="Q62" s="20"/>
+      <c r="R62" s="20"/>
       <c r="S62" s="14"/>
       <c r="T62"/>
     </row>
-    <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>296</v>
-      </c>
-      <c r="B63" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" t="s">
-        <v>298</v>
-      </c>
-      <c r="D63" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" t="s">
-        <v>299</v>
+    <row r="63" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D63" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G63" s="14"/>
       <c r="M63" s="14"/>
       <c r="S63" s="14"/>
       <c r="T63"/>
     </row>
-    <row r="64" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A64" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D64" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>292</v>
-      </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="16"/>
-      <c r="N64" s="11"/>
-      <c r="O64" s="11"/>
-      <c r="P64" s="11"/>
-      <c r="Q64" s="11"/>
-      <c r="R64" s="11"/>
-      <c r="S64" s="16"/>
-    </row>
-    <row r="65" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A65" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="D65" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>19</v>
+    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>295</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
+        <v>297</v>
+      </c>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>303</v>
+      </c>
+      <c r="G64" s="14"/>
+      <c r="M64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64"/>
+    </row>
+    <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>296</v>
+      </c>
+      <c r="B65" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" t="s">
+        <v>298</v>
+      </c>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>299</v>
       </c>
       <c r="G65" s="14"/>
       <c r="M65" s="14"/>
       <c r="S65" s="14"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D66" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="G66" s="14"/>
-      <c r="M66" s="14"/>
-      <c r="S66" s="14"/>
-      <c r="T66"/>
-    </row>
-    <row r="67" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>290</v>
-      </c>
-      <c r="B67" t="s">
-        <v>5</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="D67" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>4</v>
+    <row r="66" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D66" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="G66" s="16"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="K66" s="11"/>
+      <c r="L66" s="11"/>
+      <c r="M66" s="16"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="16"/>
+    </row>
+    <row r="67" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D67" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G67" s="14"/>
       <c r="M67" s="14"/>
       <c r="S67" s="14"/>
       <c r="T67"/>
     </row>
-    <row r="68" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D68" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>220</v>
+    <row r="68" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>209</v>
       </c>
       <c r="G68" s="14"/>
       <c r="M68" s="14"/>
       <c r="S68" s="14"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>262</v>
+        <v>290</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
-      </c>
-      <c r="C69" t="s">
-        <v>263</v>
-      </c>
-      <c r="D69" t="b">
+        <v>5</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="D69" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E69" t="b">
         <v>1</v>
       </c>
-      <c r="F69" t="s">
-        <v>228</v>
+      <c r="F69" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G69" s="14"/>
       <c r="M69" s="14"/>
       <c r="S69" s="14"/>
       <c r="T69"/>
     </row>
-    <row r="70" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D70" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>212</v>
+    <row r="70" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A70" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D70" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="G70" s="14"/>
       <c r="M70" s="14"/>
       <c r="S70" s="14"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>328</v>
+    <row r="71" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>262</v>
+      </c>
+      <c r="B71" t="s">
+        <v>82</v>
+      </c>
+      <c r="C71" t="s">
+        <v>263</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>228</v>
       </c>
       <c r="G71" s="14"/>
       <c r="M71" s="14"/>
@@ -3578,46 +3678,46 @@
     </row>
     <row r="72" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
-        <v>193</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>194</v>
+        <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>195</v>
+        <v>148</v>
       </c>
       <c r="D72" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E72" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G72" s="14"/>
       <c r="M72" s="14"/>
       <c r="S72" s="14"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
-        <v>254</v>
+        <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>256</v>
+        <v>72</v>
       </c>
       <c r="D73" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E73" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>255</v>
+        <v>328</v>
       </c>
       <c r="G73" s="14"/>
       <c r="M73" s="14"/>
@@ -3626,109 +3726,112 @@
     </row>
     <row r="74" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>10</v>
+        <v>194</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>74</v>
+        <v>195</v>
       </c>
       <c r="D74" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="G74" s="14"/>
-      <c r="H74" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K74" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="M74" s="14"/>
-      <c r="N74" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P74" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R74" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="S74" s="14"/>
       <c r="T74"/>
     </row>
     <row r="75" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
-        <v>196</v>
+        <v>254</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>289</v>
+        <v>256</v>
       </c>
       <c r="D75" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E75" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="G75" s="14"/>
       <c r="M75" s="14"/>
       <c r="S75" s="14"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D76" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>16</v>
+    <row r="76" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A76" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G76" s="14"/>
+      <c r="H76" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>307</v>
+      </c>
       <c r="M76" s="14"/>
+      <c r="N76" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P76" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="R76" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="S76" s="14"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>300</v>
+        <v>196</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>301</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="D77" s="1" t="b">
         <v>0</v>
@@ -3736,228 +3839,195 @@
       <c r="E77" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G77" s="14"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
       <c r="M77" s="14"/>
-      <c r="N77" s="1"/>
-      <c r="O77" s="1"/>
-      <c r="P77" s="1"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
       <c r="S77" s="14"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>219</v>
+        <v>337</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>231</v>
+        <v>338</v>
       </c>
       <c r="D78" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>16</v>
+        <v>228</v>
       </c>
       <c r="G78" s="14"/>
       <c r="M78" s="14"/>
       <c r="S78" s="14"/>
-      <c r="T78"/>
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>77</v>
+        <v>339</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>5</v>
+        <v>335</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>78</v>
+        <v>336</v>
       </c>
       <c r="D79" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E79" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>4</v>
+        <v>340</v>
       </c>
       <c r="G79" s="14"/>
       <c r="M79" s="14"/>
       <c r="S79" s="14"/>
-      <c r="T79"/>
-    </row>
-    <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="80" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>341</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>342</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>80</v>
+        <v>343</v>
       </c>
       <c r="D80" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>344</v>
       </c>
       <c r="G80" s="14"/>
-      <c r="H80" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K80" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="L80" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="M80" s="14"/>
-      <c r="N80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="O80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R80" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="S80" s="14"/>
-      <c r="T80"/>
-    </row>
-    <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A81" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D81" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E81" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>149</v>
+    </row>
+    <row r="81" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B81" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D81" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E81" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G81" s="14"/>
       <c r="M81" s="14"/>
       <c r="S81" s="14"/>
       <c r="T81"/>
     </row>
-    <row r="82" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A82" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D82" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>306</v>
+    <row r="82" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A82" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D82" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G82" s="14"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
       <c r="M82" s="14"/>
+      <c r="N82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
       <c r="S82" s="14"/>
       <c r="T82"/>
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>198</v>
+        <v>5</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="D83" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G83" s="14"/>
       <c r="M83" s="14"/>
       <c r="S83" s="14"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A84" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D84" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>213</v>
+    <row r="84" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A84" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G84" s="14"/>
       <c r="M84" s="14"/>
       <c r="S84" s="14"/>
       <c r="T84"/>
     </row>
-    <row r="85" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>1</v>
@@ -3967,158 +4037,144 @@
       </c>
       <c r="G85" s="14"/>
       <c r="H85" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M85" s="14"/>
       <c r="N85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R85" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S85" s="14"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D86" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="G86" s="14"/>
       <c r="M86" s="14"/>
       <c r="S86" s="14"/>
       <c r="T86"/>
     </row>
-    <row r="87" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>94</v>
+        <v>10</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D87" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>93</v>
+        <v>306</v>
       </c>
       <c r="G87" s="14"/>
       <c r="M87" s="14"/>
       <c r="S87" s="14"/>
       <c r="T87"/>
     </row>
-    <row r="88" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A88" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D88" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E88" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>16</v>
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A88" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G88" s="14"/>
       <c r="M88" s="14"/>
       <c r="S88" s="14"/>
       <c r="T88"/>
     </row>
-    <row r="89" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="D89" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E89" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F89" s="18" t="s">
-        <v>16</v>
+    <row r="89" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A89" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D89" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="G89" s="14"/>
-      <c r="H89" s="18"/>
-      <c r="I89" s="18"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="18"/>
-      <c r="L89" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M89" s="19"/>
-      <c r="N89" s="18"/>
-      <c r="O89" s="18"/>
-      <c r="P89" s="18"/>
-      <c r="Q89" s="18"/>
-      <c r="R89" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="M89" s="14"/>
       <c r="S89" s="14"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D90" s="1" t="b">
         <v>1</v>
@@ -4126,151 +4182,169 @@
       <c r="E90" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F90" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="G90" s="14"/>
+      <c r="H90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="I90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="L90" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="M90" s="14"/>
+      <c r="N90" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="P90" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q90" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="S90" s="14"/>
       <c r="T90"/>
     </row>
     <row r="91" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B91" s="6"/>
-      <c r="C91" s="6"/>
+        <v>88</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D91" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F91" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="G91" s="14"/>
-      <c r="H91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L91" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M91" s="14"/>
-      <c r="N91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O91" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R91" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S91" s="14"/>
       <c r="T91"/>
     </row>
-    <row r="92" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E92" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>4</v>
+    <row r="92" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A92" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D92" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E92" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="G92" s="14"/>
       <c r="M92" s="14"/>
       <c r="S92" s="14"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D93" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>269</v>
+    <row r="93" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A93" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D93" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G93" s="14"/>
       <c r="M93" s="14"/>
       <c r="S93" s="14"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A94" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E94" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>252</v>
+    <row r="94" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A94" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="D94" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E94" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="G94" s="14"/>
-      <c r="M94" s="14"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M94" s="19"/>
+      <c r="N94" s="18"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="18"/>
+      <c r="R94" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="S94" s="14"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>249</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>250</v>
+        <v>98</v>
       </c>
       <c r="D95" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>251</v>
+        <v>0</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="G95" s="14"/>
       <c r="M95" s="14"/>
@@ -4279,71 +4353,93 @@
     </row>
     <row r="96" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B96" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" t="s">
-        <v>278</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
       <c r="D96" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F96" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="G96" s="14"/>
+      <c r="H96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M96" s="14"/>
+      <c r="N96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S96" s="14"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
-        <v>276</v>
-      </c>
-      <c r="B97" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" t="s">
-        <v>277</v>
-      </c>
-      <c r="D97" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" t="s">
-        <v>25</v>
+    <row r="97" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G97" s="14"/>
       <c r="M97" s="14"/>
       <c r="S97" s="14"/>
       <c r="T97"/>
-      <c r="U97"/>
-    </row>
-    <row r="98" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="98" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D98" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>16</v>
+        <v>269</v>
       </c>
       <c r="G98" s="14"/>
       <c r="M98" s="14"/>
@@ -4352,13 +4448,13 @@
     </row>
     <row r="99" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>103</v>
+        <v>202</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>56</v>
+        <v>203</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="D99" s="1" t="b">
         <v>0</v>
@@ -4366,8 +4462,8 @@
       <c r="E99" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F99" s="4" t="s">
-        <v>214</v>
+      <c r="F99" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="G99" s="14"/>
       <c r="M99" s="14"/>
@@ -4376,13 +4472,13 @@
     </row>
     <row r="100" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>105</v>
+        <v>248</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>5</v>
+        <v>249</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>106</v>
+        <v>250</v>
       </c>
       <c r="D100" s="1" t="b">
         <v>0</v>
@@ -4390,8 +4486,8 @@
       <c r="E100" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F100" s="1" t="s">
-        <v>16</v>
+      <c r="F100" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="G100" s="14"/>
       <c r="M100" s="14"/>
@@ -4400,166 +4496,140 @@
     </row>
     <row r="101" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>206</v>
+        <v>222</v>
+      </c>
+      <c r="B101" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101" t="s">
+        <v>278</v>
       </c>
       <c r="D101" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G101" s="14"/>
       <c r="M101" s="14"/>
       <c r="S101" s="14"/>
       <c r="T101"/>
     </row>
-    <row r="102" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D102" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>108</v>
+    <row r="102" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>276</v>
+      </c>
+      <c r="B102" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102" t="s">
+        <v>277</v>
+      </c>
+      <c r="D102" t="b">
+        <v>1</v>
+      </c>
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" t="s">
+        <v>306</v>
       </c>
       <c r="G102" s="14"/>
       <c r="M102" s="14"/>
       <c r="S102" s="14"/>
       <c r="T102"/>
-    </row>
-    <row r="103" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="U102"/>
+    </row>
+    <row r="103" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D103" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="14"/>
-      <c r="H103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K103" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="L103" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="M103" s="14"/>
-      <c r="N103" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="O103" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P103" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q103" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R103" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="S103" s="14"/>
       <c r="T103"/>
     </row>
-    <row r="104" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C104" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D104" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E104" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>220</v>
+    <row r="104" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D104" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E104" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G104" s="14"/>
       <c r="M104" s="14"/>
       <c r="S104" s="14"/>
       <c r="T104"/>
     </row>
-    <row r="105" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C105" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D105" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E105" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F105" s="5" t="s">
-        <v>220</v>
+    <row r="105" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A105" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G105" s="14"/>
       <c r="M105" s="14"/>
       <c r="S105" s="14"/>
       <c r="T105"/>
     </row>
-    <row r="106" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A106" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B106" s="5" t="s">
+    <row r="106" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A106" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B106" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C106" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D106" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E106" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>16</v>
+      <c r="C106" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E106" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
@@ -4568,175 +4638,121 @@
     </row>
     <row r="107" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>5</v>
+        <v>109</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D107" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G107" s="14"/>
-      <c r="H107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L107" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M107" s="14"/>
-      <c r="N107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q107" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R107" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S107" s="14"/>
       <c r="T107"/>
     </row>
-    <row r="108" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E108" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G108" s="14"/>
       <c r="H108" s="1" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>4</v>
+        <v>307</v>
       </c>
       <c r="M108" s="14"/>
       <c r="N108" s="1" t="s">
-        <v>4</v>
+        <v>309</v>
       </c>
       <c r="O108" s="1" t="s">
-        <v>4</v>
+        <v>309</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>4</v>
+        <v>309</v>
       </c>
       <c r="Q108" s="1" t="s">
-        <v>4</v>
+        <v>309</v>
       </c>
       <c r="R108" s="1" t="s">
-        <v>4</v>
+        <v>309</v>
       </c>
       <c r="S108" s="14"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A109" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D109" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E109" s="1" t="b">
-        <v>1</v>
+    <row r="109" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="G109" s="14"/>
-      <c r="H109" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L109" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="M109" s="14"/>
-      <c r="N109" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q109" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R109" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="S109" s="14"/>
       <c r="T109"/>
     </row>
-    <row r="110" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A110" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D110" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E110" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>4</v>
+    <row r="110" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A110" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D110" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E110" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" s="5" t="s">
+        <v>220</v>
       </c>
       <c r="G110" s="14"/>
       <c r="M110" s="14"/>
@@ -4744,73 +4760,89 @@
       <c r="T110"/>
     </row>
     <row r="111" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>279</v>
-      </c>
-      <c r="B111" t="s">
+      <c r="A111" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B111" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C111" t="s">
-        <v>280</v>
-      </c>
-      <c r="D111" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
-        <v>4</v>
+      <c r="C111" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D111" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="14"/>
-      <c r="H111"/>
-      <c r="I111"/>
-      <c r="J111"/>
-      <c r="K111"/>
-      <c r="L111"/>
-      <c r="M111" s="17"/>
-      <c r="N111"/>
-      <c r="O111"/>
-      <c r="P111"/>
-      <c r="Q111"/>
-      <c r="R111"/>
-      <c r="S111" s="17"/>
+      <c r="M111" s="14"/>
+      <c r="S111" s="14"/>
       <c r="T111"/>
-      <c r="U111"/>
-    </row>
-    <row r="112" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A112" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C112" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D112" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E112" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>16</v>
+    </row>
+    <row r="112" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D112" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E112" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G112" s="14"/>
+      <c r="H112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M112" s="14"/>
+      <c r="N112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q112" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R112" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S112" s="14"/>
       <c r="T112"/>
     </row>
-    <row r="113" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D113" s="1" t="b">
         <v>1</v>
@@ -4820,7 +4852,7 @@
       </c>
       <c r="G113" s="14"/>
       <c r="H113" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>4</v>
@@ -4836,7 +4868,7 @@
       </c>
       <c r="M113" s="14"/>
       <c r="N113" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="O113" s="1" t="s">
         <v>4</v>
@@ -4853,18 +4885,18 @@
       <c r="S113" s="14"/>
       <c r="T113"/>
     </row>
-    <row r="114" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>240</v>
+        <v>123</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D114" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114" s="1" t="b">
         <v>1</v>
@@ -4904,127 +4936,312 @@
       <c r="S114" s="14"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>319</v>
+        <v>154</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>320</v>
+        <v>155</v>
       </c>
       <c r="D115" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F115" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G115" s="14"/>
-      <c r="H115" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="I115" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J115" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="K115" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="L115" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="M115" s="14"/>
-      <c r="N115" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="O115" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="P115" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q115" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R115" s="1" t="s">
-        <v>309</v>
-      </c>
       <c r="S115" s="14"/>
-    </row>
-    <row r="116" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A116" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B116" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D116" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E116" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F116" s="1" t="s">
-        <v>306</v>
+      <c r="T115"/>
+    </row>
+    <row r="116" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>279</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>280</v>
+      </c>
+      <c r="D116" t="b">
+        <v>0</v>
+      </c>
+      <c r="E116" t="b">
+        <v>1</v>
+      </c>
+      <c r="F116" t="s">
+        <v>4</v>
       </c>
       <c r="G116" s="14"/>
-      <c r="M116" s="14"/>
-      <c r="S116" s="14"/>
+      <c r="H116"/>
+      <c r="I116"/>
+      <c r="J116"/>
+      <c r="K116"/>
+      <c r="L116"/>
+      <c r="M116" s="17"/>
+      <c r="N116"/>
+      <c r="O116"/>
+      <c r="P116"/>
+      <c r="Q116"/>
+      <c r="R116"/>
+      <c r="S116" s="17"/>
       <c r="T116"/>
-    </row>
-    <row r="117" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A117" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="D117" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>259</v>
+      <c r="U116"/>
+    </row>
+    <row r="117" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A117" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D117" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G117" s="14"/>
       <c r="M117" s="14"/>
       <c r="S117" s="14"/>
       <c r="T117"/>
     </row>
-    <row r="118" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D118" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E118" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>228</v>
+        <v>1</v>
       </c>
       <c r="G118" s="14"/>
+      <c r="H118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M118" s="14"/>
+      <c r="N118" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R118" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S118" s="14"/>
       <c r="T118"/>
+    </row>
+    <row r="119" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A119" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D119" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E119" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G119" s="14"/>
+      <c r="H119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M119" s="14"/>
+      <c r="N119" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R119" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S119" s="14"/>
+      <c r="T119"/>
+    </row>
+    <row r="120" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A120" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D120" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G120" s="14"/>
+      <c r="H120" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I120" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J120" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L120" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="M120" s="14"/>
+      <c r="N120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="O120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="R120" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="S120" s="14"/>
+    </row>
+    <row r="121" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D121" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G121" s="14"/>
+      <c r="M121" s="14"/>
+      <c r="S121" s="14"/>
+      <c r="T121"/>
+    </row>
+    <row r="122" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A122" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G122" s="14"/>
+      <c r="M122" s="14"/>
+      <c r="S122" s="14"/>
+      <c r="T122"/>
+    </row>
+    <row r="123" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A123" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D123" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E123" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G123" s="14"/>
+      <c r="M123" s="14"/>
+      <c r="S123" s="14"/>
+      <c r="T123"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5032,10 +5249,10 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
MIM: Alias toegevoegd aan docrules.
Dit wordt opgenomen als "Alias" in de eigenschappen van alle elementen
waar deze is gespecificeerd. Dus alleen bij de documentatie die
gebaseerd is op de MIM (1.1 en hoger) regels.

Tevens MIM12 docrules overgenomen.
EIGENAAR volgt vanaf nu deze MIM regels.

Minor, verbetering.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668AEF06-E835-45B4-AC63-EB3DD03E3CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1955E3B-E9EE-4AA2-AEFD-E0652A28395F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,9 +1045,6 @@
     <t>mimformattype</t>
   </si>
   <si>
-    <t>xml</t>
-  </si>
-  <si>
     <t>mimformatversion</t>
   </si>
   <si>
@@ -1091,6 +1088,9 @@
   </si>
   <si>
     <t>STC-EIGENAAR</t>
+  </si>
+  <si>
+    <t>turtle</t>
   </si>
 </sst>
 </file>
@@ -1566,10 +1566,10 @@
   <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F108" sqref="F108"/>
+      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1810,13 +1810,13 @@
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="D9" s="1" t="b">
         <v>0</v>
@@ -2426,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G33" s="14"/>
       <c r="M33" s="14"/>
@@ -2656,13 +2656,13 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>351</v>
       </c>
       <c r="D41" s="18" t="b">
         <v>0</v>
@@ -3501,22 +3501,22 @@
     </row>
     <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
       <c r="C74" t="s">
+        <v>347</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
         <v>348</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" t="s">
-        <v>349</v>
       </c>
       <c r="G74" s="14"/>
       <c r="M74" s="14"/>
@@ -3731,7 +3731,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
@@ -3739,22 +3739,22 @@
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="D83" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D83" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="G83" s="14"/>
       <c r="M83" s="14"/>
@@ -4431,22 +4431,22 @@
     </row>
     <row r="108" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C108" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D108" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E108" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F108" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="D108" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E108" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="G108" s="14"/>
       <c r="M108" s="14"/>

</xml_diff>

<commit_message>
EIGENAAR: skos en office parameters bijgewerkt.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1955E3B-E9EE-4AA2-AEFD-E0652A28395F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5579A32B-8D5A-463E-BB90-F83B37AB53F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1566,10 +1566,10 @@
   <dimension ref="A1:U127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B61" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Panzoomimage ingesteld voor fictieve EIGENAAR
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E804878-1F69-4E0B-B3FC-64B573984B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A55EE-27DA-4651-8E32-5289213CCDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="366">
   <si>
     <t>Name</t>
   </si>
@@ -1599,10 +1599,10 @@
   <dimension ref="A1:U132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35:L35"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2405,9 +2405,6 @@
         <v>4</v>
       </c>
       <c r="G31" s="14"/>
-      <c r="H31" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M31" s="14"/>
       <c r="N31" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
EIGENAAR: nu documentor output by default
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9A55EE-27DA-4651-8E32-5289213CCDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277D4B0A-D9ED-49FF-999B-26C0D03C8951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="365">
   <si>
     <t>Name</t>
   </si>
@@ -847,9 +847,6 @@
     <t>Specify the type of office file. Multiple formats are allowed, separate list by whitespace.</t>
   </si>
   <si>
-    <t>respec msword</t>
-  </si>
-  <si>
     <t>createskos</t>
   </si>
   <si>
@@ -985,9 +982,6 @@
     <t>Name of the visuals file</t>
   </si>
   <si>
-    <t>respec</t>
-  </si>
-  <si>
     <t>fullrespec</t>
   </si>
   <si>
@@ -1124,6 +1118,9 @@
   </si>
   <si>
     <t>Vetsion of the extension. When this is a MIM model, specify the MIM extension version</t>
+  </si>
+  <si>
+    <t>documentor msword</t>
   </si>
 </sst>
 </file>
@@ -1599,10 +1596,10 @@
   <dimension ref="A1:U132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1687,35 +1684,35 @@
       <c r="F2" s="2"/>
       <c r="G2" s="13"/>
       <c r="H2" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>312</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M2" s="13"/>
       <c r="N2" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="S2" s="13"/>
       <c r="T2"/>
@@ -1843,13 +1840,13 @@
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D9" s="1" t="b">
         <v>0</v>
@@ -2103,7 +2100,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G19" s="14"/>
       <c r="M19" s="14"/>
@@ -2148,7 +2145,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G21" s="14"/>
       <c r="M21" s="14"/>
@@ -2172,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G22" s="14"/>
       <c r="M22" s="14"/>
@@ -2310,13 +2307,13 @@
     </row>
     <row r="28" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D28" s="1" t="b">
         <v>0</v>
@@ -2339,13 +2336,13 @@
     </row>
     <row r="29" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="D29" s="1" t="b">
         <v>0</v>
@@ -2456,7 +2453,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G33" s="14"/>
       <c r="M33" s="14"/>
@@ -2465,13 +2462,13 @@
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D34" s="1" t="b">
         <v>0</v>
@@ -2569,7 +2566,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G37" s="14"/>
       <c r="M37" s="14"/>
@@ -2593,40 +2590,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>273</v>
+        <v>364</v>
       </c>
       <c r="G38" s="14"/>
-      <c r="H38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="J38" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="M38" s="14"/>
-      <c r="N38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>319</v>
-      </c>
       <c r="S38" s="14"/>
       <c r="T38"/>
     </row>
@@ -2656,13 +2623,13 @@
     </row>
     <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>274</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>275</v>
       </c>
       <c r="D40" s="18" t="b">
         <v>0</v>
@@ -2692,13 +2659,13 @@
     </row>
     <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="18" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B41" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D41" s="18" t="b">
         <v>0</v>
@@ -3169,13 +3136,13 @@
     </row>
     <row r="61" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D61" s="1" t="b">
         <v>0</v>
@@ -3198,13 +3165,13 @@
     </row>
     <row r="62" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A62" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D62" s="11" t="b">
         <v>0</v>
@@ -3229,22 +3196,22 @@
     </row>
     <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="D63" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="5" t="s">
         <v>285</v>
-      </c>
-      <c r="D63" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>286</v>
       </c>
       <c r="G63" s="14"/>
       <c r="M63" s="14"/>
@@ -3253,13 +3220,13 @@
     </row>
     <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D64" s="5" t="b">
         <v>0</v>
@@ -3306,13 +3273,13 @@
     </row>
     <row r="66" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B66" t="s">
         <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D66" t="b">
         <v>0</v>
@@ -3321,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="F66" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G66" s="14"/>
       <c r="M66" s="14"/>
@@ -3330,22 +3297,22 @@
     </row>
     <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B67" t="s">
         <v>82</v>
       </c>
       <c r="C67" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
         <v>298</v>
-      </c>
-      <c r="D67" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>299</v>
       </c>
       <c r="G67" s="14"/>
       <c r="M67" s="14"/>
@@ -3369,7 +3336,7 @@
         <v>1</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G68" s="16"/>
       <c r="H68" s="11"/>
@@ -3435,13 +3402,13 @@
     </row>
     <row r="71" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
+        <v>289</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>290</v>
-      </c>
-      <c r="B71" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>291</v>
       </c>
       <c r="D71" s="1" t="b">
         <v>0</v>
@@ -3507,13 +3474,13 @@
     </row>
     <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D74" t="b">
         <v>0</v>
@@ -3522,7 +3489,7 @@
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G74" s="14"/>
       <c r="M74" s="14"/>
@@ -3570,7 +3537,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G76" s="14"/>
       <c r="M76" s="14"/>
@@ -3648,13 +3615,13 @@
     </row>
     <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D80" s="1" t="b">
         <v>0</v>
@@ -3663,7 +3630,7 @@
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G80" s="14"/>
       <c r="M80" s="14"/>
@@ -3672,13 +3639,13 @@
     </row>
     <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D81" s="1" t="b">
         <v>0</v>
@@ -3687,7 +3654,7 @@
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G81" s="14"/>
       <c r="M81" s="14"/>
@@ -3696,13 +3663,13 @@
     </row>
     <row r="82" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D82" s="1" t="b">
         <v>0</v>
@@ -3712,48 +3679,48 @@
       </c>
       <c r="G82" s="14"/>
       <c r="H82" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="M82" s="14"/>
       <c r="N82" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="P82" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="R82" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="S82" s="14"/>
       <c r="T82"/>
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>242</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D83" s="1" t="b">
         <v>0</v>
@@ -3774,7 +3741,7 @@
         <v>10</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D84" s="1" t="b">
         <v>0</v>
@@ -3789,13 +3756,13 @@
     </row>
     <row r="85" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>0</v>
@@ -3812,13 +3779,13 @@
     </row>
     <row r="86" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D86" s="1" t="b">
         <v>0</v>
@@ -3827,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G86" s="14"/>
       <c r="M86" s="14"/>
@@ -3835,22 +3802,22 @@
     </row>
     <row r="87" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="D87" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="D87" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="G87" s="14"/>
       <c r="M87" s="14"/>
@@ -3882,13 +3849,13 @@
     </row>
     <row r="89" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="D89" s="1" t="b">
         <v>0</v>
@@ -4024,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G94" s="14"/>
       <c r="M94" s="14"/>
@@ -4097,35 +4064,35 @@
       </c>
       <c r="G97" s="14"/>
       <c r="H97" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="M97" s="14"/>
       <c r="N97" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O97" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P97" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q97" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R97" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="S97" s="14"/>
       <c r="T97"/>
@@ -4204,13 +4171,13 @@
     </row>
     <row r="101" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="18" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B101" s="18" t="s">
         <v>5</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D101" s="18" t="b">
         <v>0</v>
@@ -4406,7 +4373,7 @@
         <v>10</v>
       </c>
       <c r="C108" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>1</v>
@@ -4424,13 +4391,13 @@
     </row>
     <row r="109" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D109" s="1" t="b">
         <v>0</v>
@@ -4448,13 +4415,13 @@
     </row>
     <row r="110" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B110" t="s">
         <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D110" t="b">
         <v>1</v>
@@ -4463,7 +4430,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G110" s="14"/>
       <c r="M110" s="14"/>
@@ -4521,13 +4488,13 @@
     </row>
     <row r="113" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D113" s="1" t="b">
         <v>0</v>
@@ -4536,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G113" s="14"/>
       <c r="M113" s="14"/>
@@ -4809,13 +4776,13 @@
     </row>
     <row r="125" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
+        <v>278</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
         <v>279</v>
-      </c>
-      <c r="B125" t="s">
-        <v>5</v>
-      </c>
-      <c r="C125" t="s">
-        <v>280</v>
       </c>
       <c r="D125" t="b">
         <v>0</v>
@@ -4928,13 +4895,13 @@
     </row>
     <row r="129" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D129" s="1" t="b">
         <v>0</v>
@@ -4963,7 +4930,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G130" s="14"/>
       <c r="M130" s="14"/>

</xml_diff>

<commit_message>
EIGENAAR: aanpassing properties, weergave respec
Dit is nu ook beschikbaar voor logische modellen.

Improvement.
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97518D2-0683-4E19-ADC1-EA2FFABC3794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B21A24-564C-4955-9450-65DE554D4E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="2280" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EIGENAAR" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="367">
   <si>
     <t>Name</t>
   </si>
@@ -1111,7 +1111,22 @@
     <t>Vetsion of the extension. When this is a MIM model, specify the MIM extension version</t>
   </si>
   <si>
-    <t>documentor msword</t>
+    <t>documentor</t>
+  </si>
+  <si>
+    <t>createjsonconcepts</t>
+  </si>
+  <si>
+    <t>Yes if JSON concepts must be generated</t>
+  </si>
+  <si>
+    <t>jsonconceptsname</t>
+  </si>
+  <si>
+    <t>The name of the JSON concepts file generated</t>
+  </si>
+  <si>
+    <t>yea</t>
   </si>
 </sst>
 </file>
@@ -1584,13 +1599,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U131"/>
+  <dimension ref="A1:U133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E48" sqref="A48:XFD48"/>
+      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2402,13 +2417,13 @@
     </row>
     <row r="32" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
-        <v>257</v>
+        <v>362</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>258</v>
+        <v>363</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>0</v>
@@ -2417,11 +2432,20 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" s="14"/>
+      <c r="I32" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="1" t="s">
-        <v>16</v>
+      <c r="J32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="M32" s="14"/>
       <c r="S32" s="14"/>
@@ -2429,13 +2453,13 @@
     </row>
     <row r="33" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
-        <v>262</v>
+        <v>364</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>263</v>
+        <v>365</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
@@ -2444,7 +2468,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>338</v>
+        <v>299</v>
       </c>
       <c r="G33" s="14"/>
       <c r="M33" s="14"/>
@@ -2453,13 +2477,13 @@
     </row>
     <row r="34" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
-        <v>325</v>
+        <v>257</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>326</v>
+        <v>258</v>
       </c>
       <c r="D34" s="1" t="b">
         <v>0</v>
@@ -2468,27 +2492,34 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="O34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M34" s="14"/>
-      <c r="N34" s="1" t="s">
-        <v>16</v>
+      <c r="P34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="S34" s="14"/>
-    </row>
-    <row r="35" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T34"/>
+    </row>
+    <row r="35" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>262</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
+        <v>263</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>0</v>
@@ -2497,37 +2528,22 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>19</v>
+        <v>338</v>
       </c>
       <c r="G35" s="14"/>
-      <c r="H35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L35" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="M35" s="14"/>
       <c r="S35" s="14"/>
       <c r="T35"/>
     </row>
-    <row r="36" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
-        <v>167</v>
+        <v>325</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>168</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>169</v>
+        <v>326</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>0</v>
@@ -2535,20 +2551,28 @@
       <c r="E36" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F36" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G36" s="14"/>
+      <c r="H36" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M36" s="14"/>
+      <c r="N36" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S36" s="14"/>
-      <c r="T36"/>
-    </row>
-    <row r="37" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>171</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>172</v>
+        <v>37</v>
       </c>
       <c r="D37" s="1" t="b">
         <v>0</v>
@@ -2557,7 +2581,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>324</v>
+        <v>35</v>
       </c>
       <c r="G37" s="14"/>
       <c r="M37" s="14"/>
@@ -2566,22 +2590,19 @@
     </row>
     <row r="38" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
-        <v>267</v>
+        <v>167</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>268</v>
+        <v>168</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>269</v>
+        <v>169</v>
       </c>
       <c r="D38" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="G38" s="14"/>
       <c r="M38" s="14"/>
@@ -2590,13 +2611,13 @@
     </row>
     <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>5</v>
+        <v>171</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>39</v>
+        <v>172</v>
       </c>
       <c r="D39" s="1" t="b">
         <v>0</v>
@@ -2605,145 +2626,139 @@
         <v>1</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>16</v>
+        <v>324</v>
       </c>
       <c r="G39" s="14"/>
       <c r="M39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="D40" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G40" s="19"/>
-      <c r="I40" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="L40" s="18" t="s">
-        <v>4</v>
-      </c>
+    <row r="40" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="G40" s="14"/>
       <c r="M40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40"/>
     </row>
-    <row r="41" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>343</v>
-      </c>
-      <c r="D41" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="I41" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K41" s="18" t="s">
-        <v>4</v>
-      </c>
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="14"/>
       <c r="M41" s="14"/>
       <c r="S41" s="14"/>
       <c r="T41"/>
     </row>
-    <row r="42" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G42" s="14"/>
-      <c r="J42" s="1" t="s">
+    <row r="42" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="D42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="19"/>
+      <c r="I42" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="1" t="s">
+      <c r="J42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K42" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L42" s="18" t="s">
         <v>4</v>
       </c>
       <c r="M42" s="14"/>
       <c r="S42" s="14"/>
       <c r="T42"/>
     </row>
-    <row r="43" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A43" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E43" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G43" s="14"/>
+    <row r="43" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="D43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" s="19"/>
+      <c r="I43" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="K43" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="M43" s="14"/>
       <c r="S43" s="14"/>
       <c r="T43"/>
     </row>
-    <row r="44" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:20" s="1" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D44" s="1" t="b">
         <v>0</v>
@@ -2752,37 +2767,37 @@
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="14"/>
+      <c r="J44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="1" t="s">
-        <v>16</v>
+      <c r="K44" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="M44" s="14"/>
-      <c r="N44" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S44" s="14"/>
       <c r="T44"/>
     </row>
-    <row r="45" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
-        <v>261</v>
+        <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>264</v>
+        <v>43</v>
       </c>
       <c r="D45" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E45" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>265</v>
+        <v>16</v>
       </c>
       <c r="G45" s="14"/>
       <c r="M45" s="14"/>
@@ -2791,13 +2806,13 @@
     </row>
     <row r="46" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
-        <v>173</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>174</v>
+        <v>45</v>
       </c>
       <c r="D46" s="1" t="b">
         <v>0</v>
@@ -2810,27 +2825,39 @@
       </c>
       <c r="G46" s="14"/>
       <c r="M46" s="14"/>
+      <c r="O46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="S46" s="14"/>
       <c r="T46"/>
     </row>
-    <row r="47" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A47" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>16</v>
+    <row r="47" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="G47" s="14"/>
       <c r="M47" s="14"/>
@@ -2838,16 +2865,16 @@
       <c r="T47"/>
     </row>
     <row r="48" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D48" s="21" t="b">
+      <c r="A48" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D48" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="1" t="b">
@@ -2861,31 +2888,48 @@
       <c r="S48" s="14"/>
       <c r="T48"/>
     </row>
-    <row r="49" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
+    <row r="49" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A49" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="G49" s="14"/>
       <c r="M49" s="14"/>
       <c r="S49" s="14"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A50" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D50" s="1" t="b">
+    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="21" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G50" s="14"/>
       <c r="M50" s="14"/>
@@ -2893,24 +2937,10 @@
       <c r="T50"/>
     </row>
     <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
       <c r="G51" s="14"/>
       <c r="M51" s="14"/>
       <c r="S51" s="14"/>
@@ -2918,158 +2948,155 @@
     </row>
     <row r="52" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>53</v>
+        <v>176</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>54</v>
+        <v>177</v>
       </c>
       <c r="D52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G52" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="G52" s="14"/>
       <c r="M52" s="14"/>
       <c r="S52" s="14"/>
       <c r="T52"/>
     </row>
     <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="G53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="S53" s="15"/>
+      <c r="F53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="14"/>
+      <c r="M53" s="14"/>
+      <c r="S53" s="14"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D54" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G54" s="14"/>
+    <row r="54" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G54" s="15"/>
       <c r="M54" s="14"/>
       <c r="S54" s="14"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A55" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D55" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="G55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="S55" s="14"/>
+    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="S55" s="15"/>
       <c r="T55"/>
     </row>
-    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>16</v>
+    <row r="56" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="G56" s="14"/>
       <c r="M56" s="14"/>
       <c r="S56" s="14"/>
       <c r="T56"/>
     </row>
-    <row r="57" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>16</v>
+    <row r="57" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A57" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D57" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="G57" s="14"/>
       <c r="M57" s="14"/>
       <c r="S57" s="14"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F58" s="5" t="s">
+    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G58" s="14"/>
@@ -3079,13 +3106,13 @@
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>183</v>
+        <v>57</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
       <c r="D59" s="1" t="b">
         <v>0</v>
@@ -3101,137 +3128,126 @@
       <c r="S59" s="14"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" s="14"/>
+      <c r="M60" s="14"/>
+      <c r="S60" s="14"/>
+      <c r="T60"/>
+    </row>
+    <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" s="14"/>
+      <c r="M61" s="14"/>
+      <c r="S61" s="14"/>
+      <c r="T61"/>
+    </row>
+    <row r="62" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A62" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="B62" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="D62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="G60" s="14"/>
-      <c r="H60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M60" s="14"/>
-      <c r="N60" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S60" s="14"/>
-    </row>
-    <row r="61" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A61" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="D61" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="11"/>
-      <c r="G61" s="16"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-      <c r="L61" s="11"/>
-      <c r="M61" s="16"/>
-      <c r="N61" s="11"/>
-      <c r="O61" s="11"/>
-      <c r="P61" s="11"/>
-      <c r="Q61" s="11"/>
-      <c r="R61" s="11"/>
-      <c r="S61" s="16"/>
-    </row>
-    <row r="62" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D62" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="G62" s="14"/>
       <c r="M62" s="14"/>
       <c r="S62" s="14"/>
-      <c r="T62"/>
-    </row>
-    <row r="63" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="D63" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="J63" s="20"/>
-      <c r="K63" s="20"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="20"/>
-      <c r="O63" s="20"/>
-      <c r="P63" s="20"/>
-      <c r="Q63" s="20"/>
-      <c r="R63" s="20"/>
-      <c r="S63" s="14"/>
-      <c r="T63"/>
-    </row>
-    <row r="64" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="63" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A63" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D63" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="11"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="K63" s="11"/>
+      <c r="L63" s="11"/>
+      <c r="M63" s="16"/>
+      <c r="N63" s="11"/>
+      <c r="O63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="Q63" s="11"/>
+      <c r="R63" s="11"/>
+      <c r="S63" s="16"/>
+    </row>
+    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A64" s="5" t="s">
-        <v>185</v>
+        <v>279</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>157</v>
+        <v>280</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>186</v>
+        <v>281</v>
       </c>
       <c r="D64" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E64" s="5" t="b">
         <v>1</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>282</v>
       </c>
       <c r="G64" s="14"/>
       <c r="M64" s="14"/>
@@ -3239,200 +3255,205 @@
       <c r="T64"/>
     </row>
     <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>291</v>
-      </c>
-      <c r="B65" t="s">
-        <v>79</v>
-      </c>
-      <c r="C65" t="s">
-        <v>293</v>
-      </c>
-      <c r="D65" t="b">
-        <v>0</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
-      </c>
-      <c r="F65" t="s">
-        <v>299</v>
-      </c>
+      <c r="A65" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="D65" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F65" s="20"/>
       <c r="G65" s="14"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="20"/>
+      <c r="L65" s="20"/>
       <c r="M65" s="14"/>
+      <c r="N65" s="20"/>
+      <c r="O65" s="20"/>
+      <c r="P65" s="20"/>
+      <c r="Q65" s="20"/>
+      <c r="R65" s="20"/>
       <c r="S65" s="14"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>292</v>
-      </c>
-      <c r="B66" t="s">
-        <v>79</v>
-      </c>
-      <c r="C66" t="s">
-        <v>294</v>
-      </c>
-      <c r="D66" t="b">
-        <v>0</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
-      </c>
-      <c r="F66" t="s">
-        <v>295</v>
+    <row r="66" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A66" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D66" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G66" s="14"/>
       <c r="M66" s="14"/>
       <c r="S66" s="14"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A67" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="D67" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="G67" s="16"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="16"/>
-      <c r="N67" s="11"/>
-      <c r="O67" s="11"/>
-      <c r="P67" s="11"/>
-      <c r="Q67" s="11"/>
-      <c r="R67" s="11"/>
-      <c r="S67" s="16"/>
-    </row>
-    <row r="68" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A68" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D68" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>19</v>
+    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>291</v>
+      </c>
+      <c r="B67" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" t="s">
+        <v>293</v>
+      </c>
+      <c r="D67" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" t="b">
+        <v>1</v>
+      </c>
+      <c r="F67" t="s">
+        <v>299</v>
+      </c>
+      <c r="G67" s="14"/>
+      <c r="M67" s="14"/>
+      <c r="S67" s="14"/>
+      <c r="T67"/>
+    </row>
+    <row r="68" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>292</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" t="s">
+        <v>294</v>
+      </c>
+      <c r="D68" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" t="b">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>295</v>
       </c>
       <c r="G68" s="14"/>
       <c r="M68" s="14"/>
       <c r="S68" s="14"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D69" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G69" s="14"/>
-      <c r="M69" s="14"/>
-      <c r="S69" s="14"/>
-      <c r="T69"/>
-    </row>
-    <row r="70" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>286</v>
-      </c>
-      <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="D70" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" t="b">
-        <v>1</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>4</v>
+    <row r="69" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A69" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D69" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="G69" s="16"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11"/>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11"/>
+      <c r="M69" s="16"/>
+      <c r="N69" s="11"/>
+      <c r="O69" s="11"/>
+      <c r="P69" s="11"/>
+      <c r="Q69" s="11"/>
+      <c r="R69" s="11"/>
+      <c r="S69" s="16"/>
+    </row>
+    <row r="70" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G70" s="14"/>
       <c r="M70" s="14"/>
       <c r="S70" s="14"/>
       <c r="T70"/>
     </row>
-    <row r="71" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D71" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>217</v>
+    <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A71" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D71" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>206</v>
       </c>
       <c r="G71" s="14"/>
       <c r="M71" s="14"/>
       <c r="S71" s="14"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="B72" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" t="s">
-        <v>260</v>
-      </c>
-      <c r="D72" t="b">
+        <v>5</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D72" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
       </c>
-      <c r="F72" t="s">
-        <v>225</v>
+      <c r="F72" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G72" s="14"/>
       <c r="M72" s="14"/>
@@ -3440,71 +3461,71 @@
       <c r="T72"/>
     </row>
     <row r="73" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>339</v>
-      </c>
-      <c r="B73" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" t="s">
-        <v>340</v>
-      </c>
-      <c r="D73" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" t="b">
-        <v>1</v>
-      </c>
-      <c r="F73" t="s">
-        <v>341</v>
+      <c r="A73" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="G73" s="14"/>
       <c r="M73" s="14"/>
       <c r="S73" s="14"/>
       <c r="T73"/>
     </row>
-    <row r="74" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A74" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D74" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>209</v>
+    <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>259</v>
+      </c>
+      <c r="B74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" t="s">
+        <v>260</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" t="s">
+        <v>225</v>
       </c>
       <c r="G74" s="14"/>
       <c r="M74" s="14"/>
       <c r="S74" s="14"/>
       <c r="T74"/>
     </row>
-    <row r="75" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B75" s="1" t="s">
+    <row r="75" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>339</v>
+      </c>
+      <c r="B75" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E75" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>321</v>
+      <c r="C75" t="s">
+        <v>340</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
+      </c>
+      <c r="E75" t="b">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
+        <v>341</v>
       </c>
       <c r="G75" s="14"/>
       <c r="M75" s="14"/>
@@ -3513,67 +3534,70 @@
     </row>
     <row r="76" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
-        <v>190</v>
+        <v>66</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>191</v>
+        <v>67</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
       <c r="D76" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E76" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="G76" s="14"/>
       <c r="M76" s="14"/>
       <c r="S76" s="14"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>251</v>
+        <v>68</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>253</v>
+        <v>69</v>
       </c>
       <c r="D77" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E77" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>252</v>
+        <v>321</v>
       </c>
       <c r="G77" s="14"/>
       <c r="M77" s="14"/>
       <c r="S77" s="14"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>71</v>
+        <v>192</v>
       </c>
       <c r="D78" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>207</v>
       </c>
       <c r="G78" s="14"/>
       <c r="M78" s="14"/>
@@ -3582,13 +3606,13 @@
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>356</v>
+        <v>251</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>357</v>
+        <v>253</v>
       </c>
       <c r="D79" s="1" t="b">
         <v>0</v>
@@ -3597,31 +3621,28 @@
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>341</v>
+        <v>252</v>
       </c>
       <c r="G79" s="14"/>
       <c r="M79" s="14"/>
       <c r="S79" s="14"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>353</v>
+        <v>70</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>358</v>
+        <v>71</v>
       </c>
       <c r="D80" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="G80" s="14"/>
       <c r="M80" s="14"/>
@@ -3630,13 +3651,13 @@
     </row>
     <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D81" s="1" t="b">
         <v>0</v>
@@ -3644,56 +3665,32 @@
       <c r="E81" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F81" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="G81" s="14"/>
-      <c r="H81" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="I81" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="K81" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L81" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="M81" s="14"/>
-      <c r="N81" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="O81" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="P81" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q81" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="R81" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="S81" s="14"/>
       <c r="T81"/>
     </row>
     <row r="82" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D82" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E82" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>350</v>
       </c>
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
@@ -3702,13 +3699,13 @@
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>193</v>
+        <v>354</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>285</v>
+        <v>359</v>
       </c>
       <c r="D83" s="1" t="b">
         <v>0</v>
@@ -3717,65 +3714,91 @@
         <v>1</v>
       </c>
       <c r="G83" s="14"/>
+      <c r="H83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L83" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="M83" s="14"/>
+      <c r="N83" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="P83" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="S83" s="14"/>
       <c r="T83"/>
     </row>
-    <row r="84" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>329</v>
+        <v>355</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>239</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="D84" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E84" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="G84" s="14"/>
       <c r="M84" s="14"/>
       <c r="S84" s="14"/>
+      <c r="T84"/>
     </row>
     <row r="85" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>331</v>
+        <v>193</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E85" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>347</v>
       </c>
       <c r="G85" s="14"/>
       <c r="M85" s="14"/>
       <c r="S85" s="14"/>
+      <c r="T85"/>
     </row>
     <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>333</v>
+        <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D86" s="1" t="b">
         <v>0</v>
@@ -3784,45 +3807,44 @@
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>335</v>
+        <v>225</v>
       </c>
       <c r="G86" s="14"/>
       <c r="M86" s="14"/>
       <c r="S86" s="14"/>
     </row>
-    <row r="87" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D87" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E87" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>16</v>
+    <row r="87" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A87" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D87" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="G87" s="14"/>
       <c r="M87" s="14"/>
       <c r="S87" s="14"/>
-      <c r="T87"/>
-    </row>
-    <row r="88" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="88" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>296</v>
+        <v>332</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>297</v>
+        <v>333</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="D88" s="1" t="b">
         <v>0</v>
@@ -3831,40 +3853,29 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>16</v>
+        <v>335</v>
       </c>
       <c r="G88" s="14"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
       <c r="M88" s="14"/>
-      <c r="N88" s="1"/>
-      <c r="O88" s="1"/>
-      <c r="P88" s="1"/>
-      <c r="Q88" s="1"/>
-      <c r="R88" s="1"/>
       <c r="S88" s="14"/>
-      <c r="T88"/>
-    </row>
-    <row r="89" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A89" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="D89" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="1" t="s">
+    </row>
+    <row r="89" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D89" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G89" s="14"/>
@@ -3872,45 +3883,58 @@
       <c r="S89" s="14"/>
       <c r="T89"/>
     </row>
-    <row r="90" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
-        <v>74</v>
+        <v>296</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>75</v>
+        <v>298</v>
       </c>
       <c r="D90" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G90" s="14"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
       <c r="M90" s="14"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
       <c r="S90" s="14"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>76</v>
+        <v>216</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>77</v>
+        <v>228</v>
       </c>
       <c r="D91" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G91" s="14"/>
       <c r="M91" s="14"/>
@@ -3919,13 +3943,13 @@
     </row>
     <row r="92" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>79</v>
+        <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D92" s="1" t="b">
         <v>0</v>
@@ -3934,31 +3958,28 @@
         <v>0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>146</v>
+        <v>4</v>
       </c>
       <c r="G92" s="14"/>
       <c r="M92" s="14"/>
       <c r="S92" s="14"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B93" s="5" t="s">
+    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C93" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D93" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F93" s="5" t="s">
-        <v>302</v>
+      <c r="C93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D93" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E93" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G93" s="14"/>
       <c r="M93" s="14"/>
@@ -3967,13 +3988,13 @@
     </row>
     <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
-        <v>194</v>
+        <v>78</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="D94" s="1" t="b">
         <v>0</v>
@@ -3982,154 +4003,154 @@
         <v>0</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="G94" s="14"/>
       <c r="M94" s="14"/>
       <c r="S94" s="14"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A95" s="5" t="s">
-        <v>197</v>
+        <v>81</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>176</v>
+        <v>10</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="D95" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>210</v>
+        <v>302</v>
       </c>
       <c r="G95" s="14"/>
       <c r="M95" s="14"/>
       <c r="S95" s="14"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>83</v>
+        <v>194</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>10</v>
+        <v>195</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="D96" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>0</v>
       </c>
+      <c r="F96" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G96" s="14"/>
-      <c r="H96" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="K96" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="L96" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="M96" s="14"/>
-      <c r="N96" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="O96" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="P96" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q96" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="R96" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="S96" s="14"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D97" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E97" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>86</v>
+    <row r="97" spans="1:21" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A97" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="G97" s="14"/>
       <c r="M97" s="14"/>
       <c r="S97" s="14"/>
       <c r="T97"/>
     </row>
-    <row r="98" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A98" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D98" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E98" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F98" s="5" t="s">
-        <v>90</v>
+    <row r="98" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A98" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D98" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E98" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G98" s="14"/>
+      <c r="H98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="M98" s="14"/>
+      <c r="N98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="P98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q98" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="S98" s="14"/>
       <c r="T98"/>
     </row>
-    <row r="99" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A99" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D99" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E99" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F99" s="5" t="s">
-        <v>16</v>
+    <row r="99" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A99" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D99" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E99" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="G99" s="14"/>
       <c r="M99" s="14"/>
@@ -4137,123 +4158,109 @@
       <c r="T99"/>
     </row>
     <row r="100" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="B100" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C100" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="D100" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="18" t="s">
-        <v>16</v>
+      <c r="A100" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C100" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D100" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E100" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="G100" s="14"/>
-      <c r="H100" s="18"/>
-      <c r="I100" s="18"/>
-      <c r="J100" s="18"/>
-      <c r="K100" s="18"/>
-      <c r="L100" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M100" s="19"/>
-      <c r="N100" s="18"/>
-      <c r="O100" s="18"/>
-      <c r="P100" s="18"/>
-      <c r="Q100" s="18"/>
-      <c r="R100" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="M100" s="14"/>
       <c r="S100" s="14"/>
       <c r="T100"/>
     </row>
-    <row r="101" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A101" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D101" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E101" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>94</v>
+    <row r="101" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A101" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D101" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E101" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G101" s="14"/>
       <c r="M101" s="14"/>
       <c r="S101" s="14"/>
       <c r="T101"/>
     </row>
-    <row r="102" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E102" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" s="1" t="s">
+    <row r="102" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A102" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D102" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" s="14"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G102" s="14"/>
-      <c r="H102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M102" s="14"/>
-      <c r="N102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O102" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R102" s="1" t="s">
-        <v>16</v>
+      <c r="M102" s="19"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="18"/>
+      <c r="P102" s="18"/>
+      <c r="Q102" s="18"/>
+      <c r="R102" s="18" t="s">
+        <v>4</v>
       </c>
       <c r="S102" s="14"/>
       <c r="T102"/>
     </row>
-    <row r="103" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="D103" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="G103" s="14"/>
       <c r="M103" s="14"/>
@@ -4262,37 +4269,51 @@
     </row>
     <row r="104" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B104" s="6"/>
+      <c r="C104" s="6"/>
       <c r="D104" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E104" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>266</v>
+        <v>4</v>
       </c>
       <c r="G104" s="14"/>
+      <c r="H104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L104" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M104" s="14"/>
+      <c r="N104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S104" s="14"/>
       <c r="T104"/>
     </row>
-    <row r="105" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>201</v>
+        <v>150</v>
       </c>
       <c r="D105" s="1" t="b">
         <v>0</v>
@@ -4301,70 +4322,70 @@
         <v>1</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>249</v>
+        <v>4</v>
       </c>
       <c r="G105" s="14"/>
       <c r="M105" s="14"/>
       <c r="S105" s="14"/>
       <c r="T105"/>
     </row>
-    <row r="106" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>245</v>
+        <v>96</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>246</v>
+        <v>10</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>247</v>
+        <v>97</v>
       </c>
       <c r="D106" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F106" s="4" t="s">
-        <v>248</v>
+        <v>0</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
       <c r="S106" s="14"/>
       <c r="T106"/>
     </row>
-    <row r="107" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B107" t="s">
-        <v>10</v>
-      </c>
-      <c r="C107" t="s">
-        <v>274</v>
+        <v>199</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="D107" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>25</v>
+        <v>249</v>
       </c>
       <c r="G107" s="14"/>
       <c r="M107" s="14"/>
       <c r="S107" s="14"/>
       <c r="T107"/>
     </row>
-    <row r="108" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>348</v>
+        <v>245</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C108" t="s">
-        <v>349</v>
+        <v>246</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>0</v>
@@ -4372,48 +4393,47 @@
       <c r="E108" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="1" t="s">
-        <v>16</v>
+      <c r="F108" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="G108" s="14"/>
       <c r="M108" s="14"/>
       <c r="S108" s="14"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>272</v>
+    <row r="109" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="B109" t="s">
         <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
-      </c>
-      <c r="D109" t="b">
-        <v>1</v>
-      </c>
-      <c r="E109" t="b">
-        <v>1</v>
-      </c>
-      <c r="F109" t="s">
-        <v>302</v>
+        <v>274</v>
+      </c>
+      <c r="D109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G109" s="14"/>
       <c r="M109" s="14"/>
       <c r="S109" s="14"/>
       <c r="T109"/>
-      <c r="U109"/>
-    </row>
-    <row r="110" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="110" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>98</v>
+        <v>348</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>99</v>
+      <c r="C110" t="s">
+        <v>349</v>
       </c>
       <c r="D110" s="1" t="b">
         <v>0</v>
@@ -4429,39 +4449,40 @@
       <c r="S110" s="14"/>
       <c r="T110"/>
     </row>
-    <row r="111" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A111" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D111" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E111" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" s="4" t="s">
-        <v>211</v>
+    <row r="111" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>272</v>
+      </c>
+      <c r="B111" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" t="s">
+        <v>273</v>
+      </c>
+      <c r="D111" t="b">
+        <v>1</v>
+      </c>
+      <c r="E111" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" t="s">
+        <v>302</v>
       </c>
       <c r="G111" s="14"/>
       <c r="M111" s="14"/>
       <c r="S111" s="14"/>
       <c r="T111"/>
-    </row>
-    <row r="112" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="U111"/>
+    </row>
+    <row r="112" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>344</v>
+        <v>98</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>345</v>
+        <v>99</v>
       </c>
       <c r="D112" s="1" t="b">
         <v>0</v>
@@ -4469,8 +4490,8 @@
       <c r="E112" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F112" s="4" t="s">
-        <v>346</v>
+      <c r="F112" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G112" s="14"/>
       <c r="M112" s="14"/>
@@ -4479,13 +4500,13 @@
     </row>
     <row r="113" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D113" s="1" t="b">
         <v>0</v>
@@ -4493,8 +4514,8 @@
       <c r="E113" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>16</v>
+      <c r="F113" s="4" t="s">
+        <v>211</v>
       </c>
       <c r="G113" s="14"/>
       <c r="M113" s="14"/>
@@ -4503,58 +4524,61 @@
     </row>
     <row r="114" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>202</v>
+        <v>344</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>203</v>
+        <v>345</v>
       </c>
       <c r="D114" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E114" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="G114" s="14"/>
       <c r="M114" s="14"/>
       <c r="S114" s="14"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D115" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
       <c r="G115" s="14"/>
       <c r="M115" s="14"/>
       <c r="S115" s="14"/>
       <c r="T115"/>
     </row>
-    <row r="116" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
-        <v>108</v>
+        <v>202</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="D116" s="1" t="b">
         <v>0</v>
@@ -4567,48 +4591,45 @@
       <c r="S116" s="14"/>
       <c r="T116"/>
     </row>
-    <row r="117" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D117" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E117" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="5" t="s">
-        <v>217</v>
+    <row r="117" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D117" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E117" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="G117" s="14"/>
       <c r="M117" s="14"/>
       <c r="S117" s="14"/>
       <c r="T117"/>
     </row>
-    <row r="118" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A118" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C118" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D118" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E118" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F118" s="5" t="s">
-        <v>217</v>
+    <row r="118" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A118" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D118" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E118" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G118" s="14"/>
       <c r="M118" s="14"/>
@@ -4617,70 +4638,70 @@
     </row>
     <row r="119" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A119" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D119" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E119" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="G119" s="14"/>
       <c r="M119" s="14"/>
       <c r="S119" s="14"/>
       <c r="T119"/>
     </row>
-    <row r="120" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D120" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E120" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F120" s="1" t="s">
-        <v>4</v>
+    <row r="120" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A120" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D120" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E120" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="G120" s="14"/>
       <c r="M120" s="14"/>
       <c r="S120" s="14"/>
       <c r="T120"/>
     </row>
-    <row r="121" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A121" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D121" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E121" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F121" s="1" t="s">
-        <v>4</v>
+    <row r="121" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A121" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D121" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E121" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G121" s="14"/>
       <c r="M121" s="14"/>
@@ -4689,13 +4710,13 @@
     </row>
     <row r="122" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A122" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D122" s="1" t="b">
         <v>0</v>
@@ -4707,28 +4728,22 @@
         <v>4</v>
       </c>
       <c r="G122" s="14"/>
-      <c r="H122" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M122" s="14"/>
-      <c r="N122" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S122" s="14"/>
       <c r="T122"/>
     </row>
-    <row r="123" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="D123" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" s="1" t="b">
         <v>1</v>
@@ -4741,202 +4756,208 @@
       <c r="S123" s="14"/>
       <c r="T123"/>
     </row>
-    <row r="124" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>275</v>
-      </c>
-      <c r="B124" t="s">
-        <v>5</v>
-      </c>
-      <c r="C124" t="s">
-        <v>276</v>
-      </c>
-      <c r="D124" t="b">
-        <v>0</v>
-      </c>
-      <c r="E124" t="b">
-        <v>1</v>
-      </c>
-      <c r="F124" t="s">
+    <row r="124" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D124" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E124" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F124" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G124" s="14"/>
-      <c r="H124"/>
-      <c r="I124"/>
-      <c r="J124"/>
-      <c r="K124"/>
-      <c r="L124"/>
-      <c r="M124" s="17"/>
-      <c r="N124"/>
-      <c r="O124"/>
-      <c r="P124"/>
-      <c r="Q124"/>
-      <c r="R124"/>
-      <c r="S124" s="17"/>
+      <c r="H124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M124" s="14"/>
+      <c r="N124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S124" s="14"/>
       <c r="T124"/>
-      <c r="U124"/>
-    </row>
-    <row r="125" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A125" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C125" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D125" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E125" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>16</v>
+    </row>
+    <row r="125" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A125" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D125" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E125" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G125" s="14"/>
       <c r="M125" s="14"/>
       <c r="S125" s="14"/>
       <c r="T125"/>
     </row>
-    <row r="126" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A126" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D126" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E126" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" s="1" t="s">
+    <row r="126" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>275</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>276</v>
+      </c>
+      <c r="D126" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" t="s">
         <v>4</v>
       </c>
       <c r="G126" s="14"/>
-      <c r="H126" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M126" s="14"/>
-      <c r="N126" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S126" s="14"/>
+      <c r="H126"/>
+      <c r="I126"/>
+      <c r="J126"/>
+      <c r="K126"/>
+      <c r="L126"/>
+      <c r="M126" s="17"/>
+      <c r="N126"/>
+      <c r="O126"/>
+      <c r="P126"/>
+      <c r="Q126"/>
+      <c r="R126"/>
+      <c r="S126" s="17"/>
       <c r="T126"/>
-    </row>
-    <row r="127" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A127" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D127" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E127" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F127" s="1" t="s">
-        <v>4</v>
+      <c r="U126"/>
+    </row>
+    <row r="127" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A127" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D127" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E127" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G127" s="14"/>
-      <c r="H127" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M127" s="14"/>
-      <c r="N127" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S127" s="14"/>
       <c r="T127"/>
     </row>
     <row r="128" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A128" s="1" t="s">
-        <v>313</v>
+        <v>125</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>314</v>
+        <v>126</v>
       </c>
       <c r="D128" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F128" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G128" s="14"/>
+      <c r="H128" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M128" s="14"/>
+      <c r="N128" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S128" s="14"/>
+      <c r="T128"/>
     </row>
     <row r="129" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>128</v>
+        <v>237</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D129" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E129" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>302</v>
+        <v>4</v>
       </c>
       <c r="G129" s="14"/>
+      <c r="H129" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M129" s="14"/>
+      <c r="N129" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S129" s="14"/>
       <c r="T129"/>
     </row>
-    <row r="130" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>254</v>
+        <v>313</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>255</v>
+        <v>314</v>
       </c>
       <c r="D130" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F130" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="G130" s="14"/>
       <c r="M130" s="14"/>
       <c r="S130" s="14"/>
-      <c r="T130"/>
-    </row>
-    <row r="131" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    </row>
+    <row r="131" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D131" s="1" t="b">
         <v>1</v>
@@ -4945,12 +4966,60 @@
         <v>0</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="G131" s="14"/>
       <c r="M131" s="14"/>
       <c r="S131" s="14"/>
       <c r="T131"/>
+    </row>
+    <row r="132" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="A132" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D132" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E132" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="G132" s="14"/>
+      <c r="M132" s="14"/>
+      <c r="S132" s="14"/>
+      <c r="T132"/>
+    </row>
+    <row r="133" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A133" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D133" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E133" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G133" s="14"/>
+      <c r="M133" s="14"/>
+      <c r="S133" s="14"/>
+      <c r="T133"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4958,10 +5027,10 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Dashboard path property tijdelijk teruggezet
</commit_message>
<xml_diff>
--- a/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
+++ b/src/main/resources/input/EIGENAAR/props/EIGENAAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\gitprojects\Imvertor-Maven\src\main\resources\input\EIGENAAR\props\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B21A24-564C-4955-9450-65DE554D4E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40572293-28B6-4785-9261-F4417C5DD0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="20057" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="370">
   <si>
     <t>Name</t>
   </si>
@@ -1127,6 +1127,15 @@
   </si>
   <si>
     <t>yea</t>
+  </si>
+  <si>
+    <t>dashboardpath</t>
+  </si>
+  <si>
+    <t>(obsolete)</t>
+  </si>
+  <si>
+    <t>/path</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1267,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1309,6 +1318,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1599,13 +1611,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U133"/>
+  <dimension ref="A1:U134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2912,24 +2924,24 @@
       <c r="S49" s="14"/>
       <c r="T49"/>
     </row>
-    <row r="50" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>16</v>
+    <row r="50" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="D50" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>369</v>
       </c>
       <c r="G50" s="14"/>
       <c r="M50" s="14"/>
@@ -2937,69 +2949,69 @@
       <c r="T50"/>
     </row>
     <row r="51" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="21"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
+      <c r="A51" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D51" s="21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="G51" s="14"/>
       <c r="M51" s="14"/>
       <c r="S51" s="14"/>
       <c r="T51"/>
     </row>
-    <row r="52" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A52" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D52" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E52" s="1" t="b">
-        <v>0</v>
-      </c>
+    <row r="52" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
       <c r="G52" s="14"/>
       <c r="M52" s="14"/>
       <c r="S52" s="14"/>
       <c r="T52"/>
     </row>
-    <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>5</v>
+        <v>176</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>51</v>
+        <v>177</v>
       </c>
       <c r="D53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G53" s="14"/>
       <c r="M53" s="14"/>
       <c r="S53" s="14"/>
       <c r="T53"/>
     </row>
-    <row r="54" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D54" s="1" t="b">
         <v>0</v>
@@ -3007,97 +3019,97 @@
       <c r="E54" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G54" s="15"/>
+      <c r="F54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="14"/>
       <c r="M54" s="14"/>
       <c r="S54" s="14"/>
       <c r="T54"/>
     </row>
-    <row r="55" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="G55" s="15"/>
+      <c r="M55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55"/>
+    </row>
+    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55"/>
-    </row>
-    <row r="56" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="5" t="s">
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G56" s="15"/>
+      <c r="M56" s="15"/>
+      <c r="S56" s="15"/>
+      <c r="T56"/>
+    </row>
+    <row r="57" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="5" t="s">
+      <c r="B57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="D56" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E56" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F56" s="5" t="s">
+      <c r="D57" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F57" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="G56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="S56" s="14"/>
-      <c r="T56"/>
-    </row>
-    <row r="57" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A57" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D57" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="G57" s="14"/>
       <c r="M57" s="14"/>
       <c r="S57" s="14"/>
       <c r="T57"/>
     </row>
-    <row r="58" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E58" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>16</v>
+    <row r="58" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A58" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D58" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="G58" s="14"/>
       <c r="M58" s="14"/>
@@ -3106,13 +3118,13 @@
     </row>
     <row r="59" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D59" s="1" t="b">
         <v>0</v>
@@ -3128,23 +3140,23 @@
       <c r="S59" s="14"/>
       <c r="T59"/>
     </row>
-    <row r="60" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="5" t="s">
+    <row r="60" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D60" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G60" s="14"/>
@@ -3152,23 +3164,23 @@
       <c r="S60" s="14"/>
       <c r="T60"/>
     </row>
-    <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D61" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1" t="s">
+    <row r="61" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G61" s="14"/>
@@ -3176,15 +3188,15 @@
       <c r="S61" s="14"/>
       <c r="T61"/>
     </row>
-    <row r="62" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
-        <v>315</v>
+        <v>183</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>316</v>
+        <v>184</v>
       </c>
       <c r="D62" s="1" t="b">
         <v>0</v>
@@ -3193,76 +3205,76 @@
         <v>1</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G62" s="14"/>
       <c r="M62" s="14"/>
       <c r="S62" s="14"/>
-    </row>
-    <row r="63" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A63" s="11" t="s">
+      <c r="T62"/>
+    </row>
+    <row r="63" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A63" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D63" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="14"/>
+      <c r="M63" s="14"/>
+      <c r="S63" s="14"/>
+    </row>
+    <row r="64" spans="1:20" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A64" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B64" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C64" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="D63" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F63" s="11"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="16"/>
-      <c r="N63" s="11"/>
-      <c r="O63" s="11"/>
-      <c r="P63" s="11"/>
-      <c r="Q63" s="11"/>
-      <c r="R63" s="11"/>
-      <c r="S63" s="16"/>
-    </row>
-    <row r="64" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="D64" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E64" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G64" s="14"/>
-      <c r="M64" s="14"/>
-      <c r="S64" s="14"/>
-      <c r="T64"/>
+      <c r="D64" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+      <c r="L64" s="11"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="11"/>
+      <c r="O64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="11"/>
+      <c r="S64" s="16"/>
     </row>
     <row r="65" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A65" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>87</v>
+        <v>280</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D65" s="5" t="b">
         <v>0</v>
@@ -3270,31 +3282,23 @@
       <c r="E65" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="F65" s="20"/>
+      <c r="F65" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="G65" s="14"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-      <c r="K65" s="20"/>
-      <c r="L65" s="20"/>
       <c r="M65" s="14"/>
-      <c r="N65" s="20"/>
-      <c r="O65" s="20"/>
-      <c r="P65" s="20"/>
-      <c r="Q65" s="20"/>
-      <c r="R65" s="20"/>
       <c r="S65" s="14"/>
       <c r="T65"/>
     </row>
-    <row r="66" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A66" s="5" t="s">
-        <v>185</v>
+        <v>283</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>186</v>
+        <v>284</v>
       </c>
       <c r="D66" s="5" t="b">
         <v>0</v>
@@ -3302,29 +3306,37 @@
       <c r="E66" s="5" t="b">
         <v>1</v>
       </c>
+      <c r="F66" s="20"/>
       <c r="G66" s="14"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
       <c r="M66" s="14"/>
+      <c r="N66" s="20"/>
+      <c r="O66" s="20"/>
+      <c r="P66" s="20"/>
+      <c r="Q66" s="20"/>
+      <c r="R66" s="20"/>
       <c r="S66" s="14"/>
       <c r="T66"/>
     </row>
-    <row r="67" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>291</v>
-      </c>
-      <c r="B67" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" t="s">
-        <v>293</v>
-      </c>
-      <c r="D67" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
-      </c>
-      <c r="F67" t="s">
-        <v>299</v>
+    <row r="67" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A67" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="5" t="b">
+        <v>1</v>
       </c>
       <c r="G67" s="14"/>
       <c r="M67" s="14"/>
@@ -3333,13 +3345,13 @@
     </row>
     <row r="68" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B68" t="s">
         <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D68" t="b">
         <v>0</v>
@@ -3348,136 +3360,136 @@
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="G68" s="14"/>
       <c r="M68" s="14"/>
       <c r="S68" s="14"/>
       <c r="T68"/>
     </row>
-    <row r="69" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A69" s="11" t="s">
+    <row r="69" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>292</v>
+      </c>
+      <c r="B69" t="s">
+        <v>79</v>
+      </c>
+      <c r="C69" t="s">
+        <v>294</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>295</v>
+      </c>
+      <c r="G69" s="14"/>
+      <c r="M69" s="14"/>
+      <c r="S69" s="14"/>
+      <c r="T69"/>
+    </row>
+    <row r="70" spans="1:20" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A70" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B70" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C70" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="D69" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="11" t="s">
+      <c r="D70" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E70" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="G69" s="16"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-      <c r="L69" s="11"/>
-      <c r="M69" s="16"/>
-      <c r="N69" s="11"/>
-      <c r="O69" s="11"/>
-      <c r="P69" s="11"/>
-      <c r="Q69" s="11"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="16"/>
-    </row>
-    <row r="70" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A70" s="5" t="s">
+      <c r="G70" s="16"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="11"/>
+      <c r="K70" s="11"/>
+      <c r="L70" s="11"/>
+      <c r="M70" s="16"/>
+      <c r="N70" s="11"/>
+      <c r="O70" s="11"/>
+      <c r="P70" s="11"/>
+      <c r="Q70" s="11"/>
+      <c r="R70" s="11"/>
+      <c r="S70" s="16"/>
+    </row>
+    <row r="71" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A71" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B71" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E70" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F70" s="5" t="s">
+      <c r="D71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E71" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="G70" s="14"/>
-      <c r="M70" s="14"/>
-      <c r="S70" s="14"/>
-      <c r="T70"/>
-    </row>
-    <row r="71" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D71" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="G71" s="14"/>
       <c r="M71" s="14"/>
       <c r="S71" s="14"/>
       <c r="T71"/>
     </row>
-    <row r="72" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>286</v>
-      </c>
-      <c r="B72" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>287</v>
+    <row r="72" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D72" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E72" t="b">
+      <c r="E72" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>4</v>
+        <v>206</v>
       </c>
       <c r="G72" s="14"/>
       <c r="M72" s="14"/>
       <c r="S72" s="14"/>
       <c r="T72"/>
     </row>
-    <row r="73" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>217</v>
+    <row r="73" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>286</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" t="b">
+        <v>1</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G73" s="14"/>
       <c r="M73" s="14"/>
@@ -3485,23 +3497,23 @@
       <c r="T73"/>
     </row>
     <row r="74" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
-        <v>259</v>
-      </c>
-      <c r="B74" t="s">
-        <v>79</v>
-      </c>
-      <c r="C74" t="s">
-        <v>260</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" t="s">
-        <v>225</v>
+      <c r="A74" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D74" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="G74" s="14"/>
       <c r="M74" s="14"/>
@@ -3510,13 +3522,13 @@
     </row>
     <row r="75" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>339</v>
+        <v>259</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="C75" t="s">
-        <v>340</v>
+        <v>260</v>
       </c>
       <c r="D75" t="b">
         <v>0</v>
@@ -3525,46 +3537,46 @@
         <v>1</v>
       </c>
       <c r="F75" t="s">
-        <v>341</v>
+        <v>225</v>
       </c>
       <c r="G75" s="14"/>
       <c r="M75" s="14"/>
       <c r="S75" s="14"/>
       <c r="T75"/>
     </row>
-    <row r="76" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A76" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D76" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>209</v>
+    <row r="76" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>339</v>
+      </c>
+      <c r="B76" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76" t="s">
+        <v>340</v>
+      </c>
+      <c r="D76" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" t="b">
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>341</v>
       </c>
       <c r="G76" s="14"/>
       <c r="M76" s="14"/>
       <c r="S76" s="14"/>
       <c r="T76"/>
     </row>
-    <row r="77" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="D77" s="1" t="b">
         <v>0</v>
@@ -3573,31 +3585,31 @@
         <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>321</v>
+        <v>209</v>
       </c>
       <c r="G77" s="14"/>
       <c r="M77" s="14"/>
       <c r="S77" s="14"/>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
-        <v>190</v>
+        <v>68</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>191</v>
+        <v>10</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>192</v>
+        <v>69</v>
       </c>
       <c r="D78" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E78" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>207</v>
+        <v>321</v>
       </c>
       <c r="G78" s="14"/>
       <c r="M78" s="14"/>
@@ -3606,13 +3618,13 @@
     </row>
     <row r="79" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>5</v>
+        <v>191</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>253</v>
+        <v>192</v>
       </c>
       <c r="D79" s="1" t="b">
         <v>0</v>
@@ -3621,52 +3633,52 @@
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="G79" s="14"/>
       <c r="M79" s="14"/>
       <c r="S79" s="14"/>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>70</v>
+        <v>251</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>71</v>
+        <v>253</v>
       </c>
       <c r="D80" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E80" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="G80" s="14"/>
       <c r="M80" s="14"/>
       <c r="S80" s="14"/>
       <c r="T80"/>
     </row>
-    <row r="81" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
-        <v>356</v>
+        <v>70</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>357</v>
+        <v>71</v>
       </c>
       <c r="D81" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E81" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>341</v>
       </c>
       <c r="G81" s="14"/>
       <c r="M81" s="14"/>
@@ -3675,13 +3687,13 @@
     </row>
     <row r="82" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D82" s="1" t="b">
         <v>0</v>
@@ -3690,7 +3702,7 @@
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="G82" s="14"/>
       <c r="M82" s="14"/>
@@ -3699,13 +3711,13 @@
     </row>
     <row r="83" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>10</v>
+        <v>239</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D83" s="1" t="b">
         <v>0</v>
@@ -3713,50 +3725,23 @@
       <c r="E83" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F83" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="G83" s="14"/>
-      <c r="H83" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>351</v>
-      </c>
       <c r="M83" s="14"/>
-      <c r="N83" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="O83" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="P83" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q83" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="R83" s="1" t="s">
-        <v>352</v>
-      </c>
       <c r="S83" s="14"/>
       <c r="T83"/>
     </row>
     <row r="84" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D84" s="1" t="b">
         <v>0</v>
@@ -3765,19 +3750,49 @@
         <v>1</v>
       </c>
       <c r="G84" s="14"/>
+      <c r="H84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="M84" s="14"/>
+      <c r="N84" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="P84" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q84" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="R84" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="S84" s="14"/>
       <c r="T84"/>
     </row>
     <row r="85" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>193</v>
+        <v>355</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>10</v>
+        <v>239</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>285</v>
+        <v>360</v>
       </c>
       <c r="D85" s="1" t="b">
         <v>0</v>
@@ -3790,38 +3805,36 @@
       <c r="S85" s="14"/>
       <c r="T85"/>
     </row>
-    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
-        <v>329</v>
+        <v>193</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>330</v>
+        <v>285</v>
       </c>
       <c r="D86" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E86" s="1" t="b">
         <v>1</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="G86" s="14"/>
       <c r="M86" s="14"/>
       <c r="S86" s="14"/>
-    </row>
-    <row r="87" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="T86"/>
+    </row>
+    <row r="87" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>327</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D87" s="1" t="b">
         <v>0</v>
@@ -3830,21 +3843,21 @@
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>347</v>
+        <v>225</v>
       </c>
       <c r="G87" s="14"/>
       <c r="M87" s="14"/>
       <c r="S87" s="14"/>
     </row>
-    <row r="88" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="D88" s="1" t="b">
         <v>0</v>
@@ -3853,328 +3866,327 @@
         <v>1</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G88" s="14"/>
       <c r="M88" s="14"/>
       <c r="S88" s="14"/>
     </row>
-    <row r="89" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D89" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E89" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>16</v>
+    <row r="89" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D89" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="G89" s="14"/>
       <c r="M89" s="14"/>
       <c r="S89" s="14"/>
-      <c r="T89"/>
-    </row>
-    <row r="90" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A90" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D90" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E90" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F90" s="1" t="s">
+    </row>
+    <row r="90" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D90" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G90" s="14"/>
-      <c r="H90" s="1"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="L90" s="1"/>
       <c r="M90" s="14"/>
-      <c r="N90" s="1"/>
-      <c r="O90" s="1"/>
-      <c r="P90" s="1"/>
-      <c r="Q90" s="1"/>
-      <c r="R90" s="1"/>
       <c r="S90" s="14"/>
       <c r="T90"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:20" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
-        <v>216</v>
+        <v>296</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>228</v>
+        <v>298</v>
       </c>
       <c r="D91" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G91" s="14"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
       <c r="M91" s="14"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+      <c r="R91" s="1"/>
       <c r="S91" s="14"/>
       <c r="T91"/>
     </row>
     <row r="92" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
-        <v>74</v>
+        <v>216</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>75</v>
+        <v>228</v>
       </c>
       <c r="D92" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G92" s="14"/>
       <c r="M92" s="14"/>
       <c r="S92" s="14"/>
       <c r="T92"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D93" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E93" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G93" s="14"/>
       <c r="M93" s="14"/>
       <c r="S93" s="14"/>
       <c r="T93"/>
     </row>
-    <row r="94" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D94" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
       <c r="G94" s="14"/>
       <c r="M94" s="14"/>
       <c r="S94" s="14"/>
       <c r="T94"/>
     </row>
-    <row r="95" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D95" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E95" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>302</v>
+    <row r="95" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A95" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E95" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>146</v>
       </c>
       <c r="G95" s="14"/>
       <c r="M95" s="14"/>
       <c r="S95" s="14"/>
       <c r="T95"/>
     </row>
-    <row r="96" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A96" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D96" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E96" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>19</v>
+    <row r="96" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D96" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>302</v>
       </c>
       <c r="G96" s="14"/>
       <c r="M96" s="14"/>
       <c r="S96" s="14"/>
       <c r="T96"/>
     </row>
-    <row r="97" spans="1:21" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
-      <c r="A97" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="D97" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E97" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>210</v>
+    <row r="97" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A97" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E97" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G97" s="14"/>
       <c r="M97" s="14"/>
       <c r="S97" s="14"/>
       <c r="T97"/>
     </row>
-    <row r="98" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D98" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E98" s="1" t="b">
-        <v>0</v>
+    <row r="98" spans="1:21" s="5" customFormat="1" ht="43.75" x14ac:dyDescent="0.4">
+      <c r="A98" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D98" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E98" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F98" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="G98" s="14"/>
-      <c r="H98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="I98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="J98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="K98" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="L98" s="1" t="s">
-        <v>303</v>
-      </c>
       <c r="M98" s="14"/>
-      <c r="N98" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="O98" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="P98" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="Q98" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="R98" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="S98" s="14"/>
       <c r="T98"/>
     </row>
     <row r="99" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D99" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E99" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="G99" s="14"/>
+      <c r="H99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="M99" s="14"/>
+      <c r="N99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="P99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="S99" s="14"/>
       <c r="T99"/>
     </row>
-    <row r="100" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A100" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C100" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D100" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E100" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F100" s="5" t="s">
-        <v>90</v>
+    <row r="100" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A100" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D100" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E100" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="G100" s="14"/>
       <c r="M100" s="14"/>
@@ -4183,22 +4195,22 @@
     </row>
     <row r="101" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
-        <v>147</v>
+        <v>89</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="D101" s="5" t="b">
         <v>0</v>
       </c>
       <c r="E101" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="G101" s="14"/>
       <c r="M101" s="14"/>
@@ -4206,117 +4218,99 @@
       <c r="T101"/>
     </row>
     <row r="102" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A102" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="B102" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C102" s="18" t="s">
-        <v>320</v>
-      </c>
-      <c r="D102" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="E102" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="F102" s="18" t="s">
+      <c r="A102" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D102" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E102" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G102" s="14"/>
-      <c r="H102" s="18"/>
-      <c r="I102" s="18"/>
-      <c r="J102" s="18"/>
-      <c r="K102" s="18"/>
-      <c r="L102" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="M102" s="19"/>
-      <c r="N102" s="18"/>
-      <c r="O102" s="18"/>
-      <c r="P102" s="18"/>
-      <c r="Q102" s="18"/>
-      <c r="R102" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="M102" s="14"/>
       <c r="S102" s="14"/>
       <c r="T102"/>
     </row>
-    <row r="103" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
-      <c r="A103" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D103" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E103" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>94</v>
+    <row r="103" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A103" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D103" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E103" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>16</v>
       </c>
       <c r="G103" s="14"/>
-      <c r="M103" s="14"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="M103" s="19"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+      <c r="R103" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="S103" s="14"/>
       <c r="T103"/>
     </row>
-    <row r="104" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:21" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="D104" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E104" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>4</v>
+        <v>94</v>
       </c>
       <c r="G104" s="14"/>
-      <c r="H104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L104" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M104" s="14"/>
-      <c r="N104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O104" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R104" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S104" s="14"/>
       <c r="T104"/>
     </row>
     <row r="105" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>150</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="B105" s="6"/>
+      <c r="C105" s="6"/>
       <c r="D105" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="1" t="b">
         <v>1</v>
@@ -4325,52 +4319,70 @@
         <v>4</v>
       </c>
       <c r="G105" s="14"/>
+      <c r="H105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L105" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M105" s="14"/>
+      <c r="N105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S105" s="14"/>
       <c r="T105"/>
     </row>
     <row r="106" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>96</v>
+        <v>149</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="D106" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>266</v>
+        <v>4</v>
       </c>
       <c r="G106" s="14"/>
       <c r="M106" s="14"/>
       <c r="S106" s="14"/>
       <c r="T106"/>
     </row>
-    <row r="107" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>199</v>
+        <v>96</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>201</v>
+        <v>97</v>
       </c>
       <c r="D107" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="G107" s="14"/>
       <c r="M107" s="14"/>
@@ -4379,13 +4391,13 @@
     </row>
     <row r="108" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>245</v>
+        <v>199</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>247</v>
+        <v>201</v>
       </c>
       <c r="D108" s="1" t="b">
         <v>0</v>
@@ -4393,32 +4405,32 @@
       <c r="E108" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="4" t="s">
-        <v>248</v>
+      <c r="F108" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="G108" s="14"/>
       <c r="M108" s="14"/>
       <c r="S108" s="14"/>
       <c r="T108"/>
     </row>
-    <row r="109" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B109" t="s">
-        <v>10</v>
-      </c>
-      <c r="C109" t="s">
-        <v>274</v>
+        <v>245</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>247</v>
       </c>
       <c r="D109" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F109" s="1" t="s">
-        <v>25</v>
+      <c r="F109" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="G109" s="14"/>
       <c r="M109" s="14"/>
@@ -4427,86 +4439,86 @@
     </row>
     <row r="110" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>5</v>
+        <v>219</v>
+      </c>
+      <c r="B110" t="s">
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>349</v>
+        <v>274</v>
       </c>
       <c r="D110" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G110" s="14"/>
       <c r="M110" s="14"/>
       <c r="S110" s="14"/>
       <c r="T110"/>
     </row>
-    <row r="111" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>272</v>
-      </c>
-      <c r="B111" t="s">
-        <v>10</v>
+    <row r="111" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A111" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>273</v>
-      </c>
-      <c r="D111" t="b">
-        <v>1</v>
-      </c>
-      <c r="E111" t="b">
-        <v>1</v>
-      </c>
-      <c r="F111" t="s">
-        <v>302</v>
+        <v>349</v>
+      </c>
+      <c r="D111" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E111" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G111" s="14"/>
       <c r="M111" s="14"/>
       <c r="S111" s="14"/>
       <c r="T111"/>
-      <c r="U111"/>
-    </row>
-    <row r="112" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A112" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D112" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E112" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>16</v>
+    </row>
+    <row r="112" spans="1:21" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>272</v>
+      </c>
+      <c r="B112" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" t="s">
+        <v>273</v>
+      </c>
+      <c r="D112" t="b">
+        <v>1</v>
+      </c>
+      <c r="E112" t="b">
+        <v>1</v>
+      </c>
+      <c r="F112" t="s">
+        <v>302</v>
       </c>
       <c r="G112" s="14"/>
       <c r="M112" s="14"/>
       <c r="S112" s="14"/>
       <c r="T112"/>
-    </row>
-    <row r="113" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="U112"/>
+    </row>
+    <row r="113" spans="1:21" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D113" s="1" t="b">
         <v>0</v>
@@ -4514,23 +4526,23 @@
       <c r="E113" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F113" s="4" t="s">
-        <v>211</v>
+      <c r="F113" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G113" s="14"/>
       <c r="M113" s="14"/>
       <c r="S113" s="14"/>
       <c r="T113"/>
     </row>
-    <row r="114" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>344</v>
+        <v>100</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>345</v>
+        <v>101</v>
       </c>
       <c r="D114" s="1" t="b">
         <v>0</v>
@@ -4539,22 +4551,22 @@
         <v>1</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>346</v>
+        <v>211</v>
       </c>
       <c r="G114" s="14"/>
       <c r="M114" s="14"/>
       <c r="S114" s="14"/>
       <c r="T114"/>
     </row>
-    <row r="115" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>102</v>
+        <v>344</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>103</v>
+        <v>345</v>
       </c>
       <c r="D115" s="1" t="b">
         <v>0</v>
@@ -4562,29 +4574,32 @@
       <c r="E115" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>16</v>
+      <c r="F115" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="G115" s="14"/>
       <c r="M115" s="14"/>
       <c r="S115" s="14"/>
       <c r="T115"/>
     </row>
-    <row r="116" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A116" s="1" t="s">
-        <v>202</v>
+        <v>102</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>203</v>
+        <v>103</v>
       </c>
       <c r="D116" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E116" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="G116" s="14"/>
       <c r="M116" s="14"/>
@@ -4593,67 +4608,64 @@
     </row>
     <row r="117" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A117" s="1" t="s">
-        <v>104</v>
+        <v>202</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>107</v>
+        <v>203</v>
       </c>
       <c r="D117" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="G117" s="14"/>
       <c r="M117" s="14"/>
       <c r="S117" s="14"/>
       <c r="T117"/>
     </row>
-    <row r="118" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A118" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D118" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="G118" s="14"/>
       <c r="M118" s="14"/>
       <c r="S118" s="14"/>
       <c r="T118"/>
     </row>
-    <row r="119" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C119" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D119" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E119" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>217</v>
+    <row r="119" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A119" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D119" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E119" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G119" s="14"/>
       <c r="M119" s="14"/>
@@ -4662,13 +4674,13 @@
     </row>
     <row r="120" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A120" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D120" s="5" t="b">
         <v>1</v>
@@ -4686,46 +4698,46 @@
     </row>
     <row r="121" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A121" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D121" s="5" t="b">
         <v>1</v>
       </c>
       <c r="E121" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="G121" s="14"/>
       <c r="M121" s="14"/>
       <c r="S121" s="14"/>
       <c r="T121"/>
     </row>
-    <row r="122" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D122" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="E122" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>4</v>
+    <row r="122" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A122" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D122" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E122" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G122" s="14"/>
       <c r="M122" s="14"/>
@@ -4734,16 +4746,16 @@
     </row>
     <row r="123" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A123" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D123" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123" s="1" t="b">
         <v>1</v>
@@ -4758,16 +4770,16 @@
     </row>
     <row r="124" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A124" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D124" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" s="1" t="b">
         <v>1</v>
@@ -4776,25 +4788,19 @@
         <v>4</v>
       </c>
       <c r="G124" s="14"/>
-      <c r="H124" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M124" s="14"/>
-      <c r="N124" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S124" s="14"/>
       <c r="T124"/>
     </row>
-    <row r="125" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A125" s="1" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="D125" s="1" t="b">
         <v>0</v>
@@ -4806,108 +4812,108 @@
         <v>4</v>
       </c>
       <c r="G125" s="14"/>
+      <c r="H125" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M125" s="14"/>
+      <c r="N125" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S125" s="14"/>
       <c r="T125"/>
     </row>
-    <row r="126" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
+    <row r="126" spans="1:21" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A126" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D126" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E126" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G126" s="14"/>
+      <c r="M126" s="14"/>
+      <c r="S126" s="14"/>
+      <c r="T126"/>
+    </row>
+    <row r="127" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
         <v>275</v>
       </c>
-      <c r="B126" t="s">
-        <v>5</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
         <v>276</v>
       </c>
-      <c r="D126" t="b">
-        <v>0</v>
-      </c>
-      <c r="E126" t="b">
-        <v>1</v>
-      </c>
-      <c r="F126" t="s">
+      <c r="D127" t="b">
+        <v>0</v>
+      </c>
+      <c r="E127" t="b">
+        <v>1</v>
+      </c>
+      <c r="F127" t="s">
         <v>4</v>
       </c>
-      <c r="G126" s="14"/>
-      <c r="H126"/>
-      <c r="I126"/>
-      <c r="J126"/>
-      <c r="K126"/>
-      <c r="L126"/>
-      <c r="M126" s="17"/>
-      <c r="N126"/>
-      <c r="O126"/>
-      <c r="P126"/>
-      <c r="Q126"/>
-      <c r="R126"/>
-      <c r="S126" s="17"/>
-      <c r="T126"/>
-      <c r="U126"/>
-    </row>
-    <row r="127" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A127" s="5" t="s">
+      <c r="G127" s="14"/>
+      <c r="H127"/>
+      <c r="I127"/>
+      <c r="J127"/>
+      <c r="K127"/>
+      <c r="L127"/>
+      <c r="M127" s="17"/>
+      <c r="N127"/>
+      <c r="O127"/>
+      <c r="P127"/>
+      <c r="Q127"/>
+      <c r="R127"/>
+      <c r="S127" s="17"/>
+      <c r="T127"/>
+      <c r="U127"/>
+    </row>
+    <row r="128" spans="1:21" s="5" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A128" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B128" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C127" s="5" t="s">
+      <c r="C128" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D127" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E127" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F127" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G127" s="14"/>
-      <c r="M127" s="14"/>
-      <c r="S127" s="14"/>
-      <c r="T127"/>
-    </row>
-    <row r="128" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A128" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B128" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D128" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E128" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>4</v>
+      <c r="D128" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E128" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="G128" s="14"/>
-      <c r="H128" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="M128" s="14"/>
-      <c r="N128" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="S128" s="14"/>
       <c r="T128"/>
     </row>
     <row r="129" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A129" s="1" t="s">
-        <v>237</v>
+        <v>125</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D129" s="1" t="b">
         <v>1</v>
@@ -4931,95 +4937,125 @@
     </row>
     <row r="130" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A130" s="1" t="s">
-        <v>313</v>
+        <v>237</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>314</v>
+        <v>127</v>
       </c>
       <c r="D130" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="F130" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G130" s="14"/>
+      <c r="H130" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="M130" s="14"/>
+      <c r="N130" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="S130" s="14"/>
+      <c r="T130"/>
     </row>
     <row r="131" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A131" s="1" t="s">
-        <v>128</v>
+        <v>313</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>129</v>
+        <v>314</v>
       </c>
       <c r="D131" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F131" s="1" t="s">
-        <v>302</v>
+        <v>1</v>
       </c>
       <c r="G131" s="14"/>
       <c r="M131" s="14"/>
       <c r="S131" s="14"/>
-      <c r="T131"/>
-    </row>
-    <row r="132" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
+    </row>
+    <row r="132" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A132" s="1" t="s">
-        <v>254</v>
+        <v>128</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>255</v>
+        <v>129</v>
       </c>
       <c r="D132" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E132" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>256</v>
+        <v>302</v>
       </c>
       <c r="G132" s="14"/>
       <c r="M132" s="14"/>
       <c r="S132" s="14"/>
       <c r="T132"/>
     </row>
-    <row r="133" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:20" s="1" customFormat="1" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A133" s="1" t="s">
-        <v>130</v>
+        <v>254</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>132</v>
+        <v>255</v>
       </c>
       <c r="D133" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E133" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="G133" s="14"/>
       <c r="M133" s="14"/>
       <c r="S133" s="14"/>
       <c r="T133"/>
+    </row>
+    <row r="134" spans="1:20" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="A134" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D134" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E134" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="G134" s="14"/>
+      <c r="M134" s="14"/>
+      <c r="S134" s="14"/>
+      <c r="T134"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5027,10 +5063,10 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>